<commit_message>
Updated Jan 2024 Opsheet
Updated Jan 2024 Opsheet
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A2BEEA-1FF4-45CE-B1EB-BC4C4AF375BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6508CC-8A49-4598-9C86-8D58499BD039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="10" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="204">
   <si>
     <t>Course</t>
   </si>
@@ -709,6 +709,18 @@
   </si>
   <si>
     <t>Priyankshu Giri</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>2:00 PM - 4:00 PM</t>
+  </si>
+  <si>
+    <t>1) Background Of</t>
+  </si>
+  <si>
+    <t>Economics</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1860,10 +1872,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2987,13 +2995,15 @@
   <dimension ref="B1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3052,7 +3062,9 @@
       <c r="C4" s="181" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="128"/>
+      <c r="D4" s="150">
+        <v>45293</v>
+      </c>
       <c r="E4" s="128"/>
       <c r="F4" s="128"/>
       <c r="G4" s="128"/>
@@ -3064,15 +3076,17 @@
       <c r="M4" s="147"/>
       <c r="N4" s="115"/>
       <c r="O4" s="116"/>
-      <c r="Q4" s="184"/>
-      <c r="R4" s="185"/>
-      <c r="S4" s="184"/>
-      <c r="T4" s="185"/>
+      <c r="Q4" s="96"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="96"/>
+      <c r="T4" s="62"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="161"/>
       <c r="C5" s="163"/>
-      <c r="D5" s="61"/>
+      <c r="D5" s="151" t="s">
+        <v>201</v>
+      </c>
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
       <c r="G5" s="61"/>
@@ -3084,10 +3098,10 @@
       <c r="M5" s="148"/>
       <c r="N5" s="59"/>
       <c r="O5" s="60"/>
-      <c r="Q5" s="184"/>
-      <c r="R5" s="185"/>
-      <c r="S5" s="184"/>
-      <c r="T5" s="185"/>
+      <c r="Q5" s="96"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="96"/>
+      <c r="T5" s="62"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="31">
@@ -3096,7 +3110,9 @@
       <c r="C6" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="49" t="s">
+        <v>200</v>
+      </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -3108,10 +3124,10 @@
       <c r="M6" s="52"/>
       <c r="N6" s="53"/>
       <c r="O6" s="54"/>
-      <c r="Q6" s="184"/>
-      <c r="R6" s="185"/>
-      <c r="S6" s="184"/>
-      <c r="T6" s="185"/>
+      <c r="Q6" s="96"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="96"/>
+      <c r="T6" s="62"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="33">
@@ -3130,10 +3146,10 @@
       <c r="M7" s="50"/>
       <c r="N7" s="42"/>
       <c r="O7" s="43"/>
-      <c r="Q7" s="184"/>
-      <c r="R7" s="185"/>
-      <c r="S7" s="184"/>
-      <c r="T7" s="185"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="62"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="33">
@@ -3152,10 +3168,10 @@
       <c r="M8" s="50"/>
       <c r="N8" s="42"/>
       <c r="O8" s="43"/>
-      <c r="Q8" s="184"/>
-      <c r="R8" s="185"/>
-      <c r="S8" s="184"/>
-      <c r="T8" s="185"/>
+      <c r="Q8" s="96"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="96"/>
+      <c r="T8" s="62"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="33">
@@ -3228,7 +3244,9 @@
         <v>36</v>
       </c>
       <c r="C12" s="159"/>
-      <c r="D12" s="62"/>
+      <c r="D12" s="62" t="s">
+        <v>202</v>
+      </c>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
       <c r="G12" s="62"/>
@@ -3248,7 +3266,9 @@
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="135"/>
       <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
+      <c r="D13" s="62" t="s">
+        <v>203</v>
+      </c>
       <c r="E13" s="62"/>
       <c r="F13" s="62"/>
       <c r="G13" s="62"/>
@@ -5733,7 +5753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
   <dimension ref="B1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Avishek docs checked in
Avishek docs checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6508CC-8A49-4598-9C86-8D58499BD039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A662FF-BFA0-4DE5-A37C-6874767B752B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="10" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
@@ -910,7 +910,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1473,11 +1473,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1870,6 +1890,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2224,12 +2259,13 @@
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
@@ -2282,7 +2318,7 @@
   <dimension ref="B1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2995,7 +3031,7 @@
   <dimension ref="B1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3038,7 +3074,7 @@
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="157"/>
       <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
+      <c r="D3" s="190"/>
       <c r="E3" s="158"/>
       <c r="F3" s="158"/>
       <c r="G3" s="158"/>
@@ -3059,10 +3095,10 @@
       <c r="B4" s="180" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="184" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="150">
+      <c r="D4" s="145">
         <v>45293</v>
       </c>
       <c r="E4" s="128"/>
@@ -3083,8 +3119,8 @@
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="161"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="151" t="s">
+      <c r="C5" s="185"/>
+      <c r="D5" s="146" t="s">
         <v>201</v>
       </c>
       <c r="E5" s="61"/>
@@ -3107,10 +3143,10 @@
       <c r="B6" s="31">
         <v>1</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="186" t="s">
         <v>199</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="42" t="s">
         <v>200</v>
       </c>
       <c r="E6" s="39"/>
@@ -3133,9 +3169,9 @@
       <c r="B7" s="33">
         <v>2</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="42"/>
       <c r="G7" s="49"/>
       <c r="H7" s="62"/>
@@ -3155,9 +3191,9 @@
       <c r="B8" s="33">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="42"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="42"/>
       <c r="G8" s="49"/>
       <c r="H8" s="62"/>
@@ -3177,9 +3213,9 @@
       <c r="B9" s="33">
         <v>4</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="42"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="42"/>
       <c r="G9" s="49"/>
       <c r="H9" s="62"/>
@@ -3199,9 +3235,9 @@
       <c r="B10" s="33">
         <v>5</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="141"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="42"/>
       <c r="G10" s="49"/>
       <c r="H10" s="62"/>
@@ -3221,9 +3257,9 @@
       <c r="B11" s="129">
         <v>6</v>
       </c>
-      <c r="C11" s="130"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
+      <c r="C11" s="187"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="131"/>
       <c r="F11" s="132"/>
       <c r="G11" s="63"/>
       <c r="H11" s="133"/>
@@ -3243,11 +3279,11 @@
       <c r="B12" s="182" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="159"/>
+      <c r="C12" s="188"/>
       <c r="D12" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="E12" s="62"/>
+      <c r="E12" s="127"/>
       <c r="F12" s="62"/>
       <c r="G12" s="62"/>
       <c r="H12" s="62"/>
@@ -3265,11 +3301,11 @@
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="135"/>
-      <c r="C13" s="62"/>
+      <c r="C13" s="141"/>
       <c r="D13" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="E13" s="62"/>
+      <c r="E13" s="127"/>
       <c r="F13" s="62"/>
       <c r="G13" s="62"/>
       <c r="H13" s="62"/>
@@ -3287,9 +3323,9 @@
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B14" s="135"/>
-      <c r="C14" s="62"/>
+      <c r="C14" s="141"/>
       <c r="D14" s="62"/>
-      <c r="E14" s="62"/>
+      <c r="E14" s="127"/>
       <c r="F14" s="62"/>
       <c r="G14" s="62"/>
       <c r="H14" s="62"/>
@@ -3307,9 +3343,9 @@
     </row>
     <row r="15" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="137"/>
-      <c r="C15" s="138"/>
-      <c r="D15" s="138"/>
-      <c r="E15" s="138"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="139"/>
       <c r="F15" s="138"/>
       <c r="G15" s="138"/>
       <c r="H15" s="138"/>
@@ -4109,8 +4145,7 @@
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.33203125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Ops 2024 Jan checked in
Ops 2024 Jan checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A662FF-BFA0-4DE5-A37C-6874767B752B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A2E57B-9D32-4A68-89DF-B6EF3B0415C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="10" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="7" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -84,26 +84,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={4EE09740-4AB8-4767-BD8A-38F7D58F39B2}</author>
-  </authors>
-  <commentList>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{4EE09740-4AB8-4767-BD8A-38F7D58F39B2}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    1) Elasticity</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="206">
   <si>
     <t>Course</t>
   </si>
@@ -721,6 +703,12 @@
   </si>
   <si>
     <t>Economics</t>
+  </si>
+  <si>
+    <t>10:30 PM - 12:30 PM</t>
+  </si>
+  <si>
+    <t>1) Transmission of heat</t>
   </si>
 </sst>
 </file>
@@ -1802,6 +1790,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1892,20 +1883,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2246,14 +2234,6 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D12" dT="2023-11-04T08:33:38.77" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{4EE09740-4AB8-4767-BD8A-38F7D58F39B2}">
-    <text>1) Elasticity</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C90D3B1-C76E-4CE0-A4AA-1FA923F6E3CF}">
   <dimension ref="B1:C5"/>
@@ -2337,14 +2317,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="157" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="156"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="159"/>
       <c r="M2" s="97" t="s">
         <v>145</v>
       </c>
@@ -2362,18 +2342,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="164" t="s">
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="165"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="166"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="169"/>
       <c r="M3" s="62"/>
       <c r="N3" s="96"/>
       <c r="O3" s="62"/>
@@ -2381,10 +2361,10 @@
       <c r="Q3" s="62"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="162" t="s">
+      <c r="C4" s="165" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37"/>
@@ -2410,8 +2390,8 @@
       <c r="Q4" s="62"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="161"/>
-      <c r="C5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
@@ -2585,10 +2565,10 @@
       <c r="Q11" s="62"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="159" t="s">
+      <c r="B12" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="159"/>
+      <c r="C12" s="162"/>
       <c r="D12" s="94"/>
       <c r="E12" s="64"/>
       <c r="F12" s="64"/>
@@ -3030,7 +3010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C94FC2-4E02-4E43-9E5D-811D6F46FE15}">
   <dimension ref="B1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -3045,19 +3025,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="157" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="156"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
       <c r="Q2" s="98" t="s">
         <v>143</v>
       </c>
@@ -3072,30 +3052,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="190"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158"/>
-      <c r="L3" s="183"/>
-      <c r="M3" s="164"/>
-      <c r="N3" s="165"/>
-      <c r="O3" s="166"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="187"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
+      <c r="L3" s="186"/>
+      <c r="M3" s="167"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="169"/>
       <c r="Q3" s="96"/>
       <c r="R3" s="62"/>
       <c r="S3" s="96"/>
       <c r="T3" s="62"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="183" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="184" t="s">
+      <c r="C4" s="188" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="145">
@@ -3118,8 +3098,8 @@
       <c r="T4" s="62"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="161"/>
-      <c r="C5" s="185"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="189"/>
       <c r="D5" s="146" t="s">
         <v>201</v>
       </c>
@@ -3143,7 +3123,7 @@
       <c r="B6" s="31">
         <v>1</v>
       </c>
-      <c r="C6" s="186" t="s">
+      <c r="C6" s="154" t="s">
         <v>199</v>
       </c>
       <c r="D6" s="42" t="s">
@@ -3257,7 +3237,7 @@
       <c r="B11" s="129">
         <v>6</v>
       </c>
-      <c r="C11" s="187"/>
+      <c r="C11" s="155"/>
       <c r="D11" s="42"/>
       <c r="E11" s="131"/>
       <c r="F11" s="132"/>
@@ -3276,10 +3256,10 @@
       <c r="T11" s="62"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="182" t="s">
+      <c r="B12" s="185" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="188"/>
+      <c r="C12" s="190"/>
       <c r="D12" s="62" t="s">
         <v>202</v>
       </c>
@@ -3343,7 +3323,7 @@
     </row>
     <row r="15" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="137"/>
-      <c r="C15" s="189"/>
+      <c r="C15" s="156"/>
       <c r="D15" s="62"/>
       <c r="E15" s="139"/>
       <c r="F15" s="138"/>
@@ -4403,14 +4383,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="157" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="156"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="159"/>
       <c r="M2" s="125" t="s">
         <v>143</v>
       </c>
@@ -4425,28 +4405,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="164" t="s">
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="165"/>
-      <c r="J3" s="165"/>
-      <c r="K3" s="166"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="169"/>
       <c r="M3" s="96"/>
       <c r="N3" s="62"/>
       <c r="O3" s="96"/>
       <c r="P3" s="62"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="162" t="s">
+      <c r="C4" s="165" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="37"/>
@@ -4469,8 +4449,8 @@
       <c r="P4" s="62"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="161"/>
-      <c r="C5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="65"/>
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
@@ -4637,10 +4617,10 @@
       <c r="P11" s="62"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="159" t="s">
+      <c r="B12" s="162" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="159"/>
+      <c r="C12" s="162"/>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
@@ -4946,16 +4926,16 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="157" t="s">
         <v>195</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="156"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="159"/>
       <c r="O2" s="125" t="s">
         <v>143</v>
       </c>
@@ -4970,30 +4950,30 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="164" t="s">
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="167" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="165"/>
-      <c r="L3" s="165"/>
-      <c r="M3" s="166"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="168"/>
+      <c r="M3" s="169"/>
       <c r="O3" s="96"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="96"/>
       <c r="R3" s="62"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="162" t="s">
+      <c r="C4" s="165" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="128"/>
@@ -5018,8 +4998,8 @@
       <c r="R4" s="62"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="161"/>
-      <c r="C5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
@@ -5200,10 +5180,10 @@
       <c r="R11" s="62"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="167" t="s">
+      <c r="B12" s="170" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="168"/>
+      <c r="C12" s="171"/>
       <c r="D12" s="126"/>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
@@ -5281,18 +5261,18 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="18.109375" bestFit="1" customWidth="1"/>
@@ -5308,19 +5288,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="175" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="173"/>
-      <c r="D2" s="173"/>
-      <c r="E2" s="173"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="173"/>
-      <c r="H2" s="173"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="174"/>
-      <c r="K2" s="174"/>
-      <c r="L2" s="175"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="178"/>
       <c r="Q2" s="98" t="s">
         <v>143</v>
       </c>
@@ -5335,33 +5315,35 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="176"/>
-      <c r="C3" s="177"/>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="177"/>
-      <c r="G3" s="177"/>
-      <c r="H3" s="177"/>
-      <c r="I3" s="178"/>
-      <c r="J3" s="178"/>
-      <c r="K3" s="178"/>
-      <c r="L3" s="179"/>
-      <c r="M3" s="164"/>
-      <c r="N3" s="165"/>
-      <c r="O3" s="166"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="180"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="181"/>
+      <c r="K3" s="181"/>
+      <c r="L3" s="182"/>
+      <c r="M3" s="167"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="169"/>
       <c r="Q3" s="96"/>
       <c r="R3" s="62"/>
       <c r="S3" s="96"/>
       <c r="T3" s="62"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="169" t="s">
+      <c r="B4" s="172" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="171" t="s">
+      <c r="C4" s="174" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="152">
+        <v>45297</v>
+      </c>
       <c r="E4" s="152"/>
       <c r="F4" s="152"/>
       <c r="G4" s="152"/>
@@ -5385,9 +5367,11 @@
       <c r="T4" s="124"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="170"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="61"/>
+      <c r="B5" s="173"/>
+      <c r="C5" s="166"/>
+      <c r="D5" s="61" t="s">
+        <v>204</v>
+      </c>
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
       <c r="G5" s="61"/>
@@ -5417,7 +5401,9 @@
       <c r="C6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="39"/>
+      <c r="D6" s="39" t="s">
+        <v>200</v>
+      </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -5445,7 +5431,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="34"/>
-      <c r="D7" s="41"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="42"/>
       <c r="F7" s="42"/>
       <c r="G7" s="49"/>
@@ -5473,7 +5459,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="34"/>
-      <c r="D8" s="41"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="42"/>
       <c r="F8" s="42"/>
       <c r="G8" s="49"/>
@@ -5501,7 +5487,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="34"/>
-      <c r="D9" s="41"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="42"/>
       <c r="F9" s="42"/>
       <c r="G9" s="49"/>
@@ -5529,7 +5515,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="34"/>
-      <c r="D10" s="41"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="49"/>
@@ -5581,11 +5567,13 @@
       <c r="T11" s="124"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="159" t="s">
+      <c r="B12" s="162" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="159"/>
-      <c r="D12" s="62"/>
+      <c r="C12" s="162"/>
+      <c r="D12" s="62" t="s">
+        <v>205</v>
+      </c>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
       <c r="G12" s="62"/>
@@ -5780,7 +5768,6 @@
     <mergeCell ref="B2:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5813,19 +5800,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="154" t="s">
+      <c r="B2" s="157" t="s">
         <v>150</v>
       </c>
-      <c r="C2" s="155"/>
-      <c r="D2" s="155"/>
-      <c r="E2" s="155"/>
-      <c r="F2" s="155"/>
-      <c r="G2" s="155"/>
-      <c r="H2" s="155"/>
-      <c r="I2" s="155"/>
-      <c r="J2" s="155"/>
-      <c r="K2" s="155"/>
-      <c r="L2" s="156"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
+      <c r="J2" s="158"/>
+      <c r="K2" s="158"/>
+      <c r="L2" s="159"/>
       <c r="Q2" s="98" t="s">
         <v>143</v>
       </c>
@@ -5840,30 +5827,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="157"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="158"/>
-      <c r="F3" s="158"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158"/>
-      <c r="L3" s="183"/>
-      <c r="M3" s="164"/>
-      <c r="N3" s="165"/>
-      <c r="O3" s="166"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="161"/>
+      <c r="D3" s="161"/>
+      <c r="E3" s="161"/>
+      <c r="F3" s="161"/>
+      <c r="G3" s="161"/>
+      <c r="H3" s="161"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
+      <c r="L3" s="186"/>
+      <c r="M3" s="167"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="169"/>
       <c r="Q3" s="96"/>
       <c r="R3" s="62"/>
       <c r="S3" s="96"/>
       <c r="T3" s="62"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="183" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="184" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="128"/>
@@ -5890,8 +5877,8 @@
       <c r="T4" s="124"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="161"/>
-      <c r="C5" s="163"/>
+      <c r="B5" s="164"/>
+      <c r="C5" s="166"/>
       <c r="D5" s="61"/>
       <c r="E5" s="61"/>
       <c r="F5" s="61"/>
@@ -6088,10 +6075,10 @@
       <c r="T11" s="62"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="182" t="s">
+      <c r="B12" s="185" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="159"/>
+      <c r="C12" s="162"/>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>

</xml_diff>

<commit_message>
Update Ops Jan 2024
Update Ops Jan 2024
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E01D05-6D9D-4F48-9EFF-AAF049CD0B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AD8749-C693-4066-84E9-412B08181902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="2" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="10" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -84,6 +84,24 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={9021DEAC-DEF2-47BD-B58D-12E2FFC4F148}</author>
+  </authors>
+  <commentList>
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{9021DEAC-DEF2-47BD-B58D-12E2FFC4F148}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    An introduction to Management - Evolution, Concept, Definition, Features, Objectives, Scope</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="187">
   <si>
@@ -661,7 +679,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -747,6 +765,12 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1606,102 +1630,6 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1717,6 +1645,102 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2056,6 +2080,14 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E12" dT="2024-01-09T07:14:49.58" personId="{A98E9D41-33A5-4BF6-BDEF-83BD84C6E107}" id="{9021DEAC-DEF2-47BD-B58D-12E2FFC4F148}">
+    <text>An introduction to Management - Evolution, Concept, Definition, Features, Objectives, Scope</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C90D3B1-C76E-4CE0-A4AA-1FA923F6E3CF}">
   <dimension ref="B1:C5"/>
@@ -2139,14 +2171,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="119" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="114"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="121"/>
       <c r="M2" s="54" t="s">
         <v>113</v>
       </c>
@@ -2164,18 +2196,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="122" t="s">
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="131"/>
       <c r="M3" s="34"/>
       <c r="N3" s="53"/>
       <c r="O3" s="34"/>
@@ -2183,10 +2215,10 @@
       <c r="Q3" s="34"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="127" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="9"/>
@@ -2212,8 +2244,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="128"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -2387,10 +2419,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="124"/>
       <c r="D12" s="51"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -2829,11 +2861,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C94FC2-4E02-4E43-9E5D-811D6F46FE15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C94FC2-4E02-4E43-9E5D-811D6F46FE15}">
   <dimension ref="B2:T26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2848,19 +2880,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="142" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
-      <c r="H2" s="135"/>
-      <c r="I2" s="135"/>
-      <c r="J2" s="135"/>
-      <c r="K2" s="135"/>
-      <c r="L2" s="135"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
       <c r="Q2" s="34"/>
       <c r="R2" s="111" t="s">
         <v>175</v>
@@ -2869,20 +2901,20 @@
       <c r="T2" s="34"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B3" s="135"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="142"/>
+      <c r="B3" s="142"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="149"/>
+      <c r="N3" s="149"/>
+      <c r="O3" s="149"/>
       <c r="Q3" s="55" t="s">
         <v>111</v>
       </c>
@@ -2897,10 +2929,10 @@
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="150" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="143" t="s">
+      <c r="C4" s="150" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="99">
@@ -2931,8 +2963,8 @@
       <c r="T4" s="34"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5" s="143"/>
-      <c r="C5" s="143"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="150"/>
       <c r="D5" s="100" t="s">
         <v>164</v>
       </c>
@@ -3128,10 +3160,10 @@
       <c r="T11" s="34"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="124"/>
       <c r="D12" s="34" t="s">
         <v>165</v>
       </c>
@@ -3355,6 +3387,7 @@
     <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3382,40 +3415,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="144" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="144" t="s">
+      <c r="C2" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="144" t="s">
+      <c r="E2" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="144" t="s">
+      <c r="F2" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="144" t="s">
+      <c r="G2" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="144" t="s">
+      <c r="H2" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="144" t="s">
+      <c r="I2" s="112" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="144" t="s">
+      <c r="J2" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="144" t="s">
+      <c r="K2" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="144" t="s">
+      <c r="L2" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="144" t="s">
+      <c r="M2" s="112" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3442,12 +3475,12 @@
         <v>0</v>
       </c>
       <c r="I3" s="1">
-        <f>G3-H3</f>
+        <f t="shared" ref="I3:I8" si="0">G3-H3</f>
         <v>3334</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="145"/>
+      <c r="L3" s="113"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.3">
@@ -3461,7 +3494,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1">
-        <f>G4-H4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="1"/>
@@ -3480,7 +3513,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1">
-        <f>G5-H5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="1"/>
@@ -3511,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f>G6-H6</f>
+        <f t="shared" si="0"/>
         <v>3333</v>
       </c>
       <c r="J6" s="1"/>
@@ -3530,7 +3563,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1">
-        <f>G7-H7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J7" s="1"/>
@@ -3549,7 +3582,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <f>G8-H8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="1"/>
@@ -3580,12 +3613,12 @@
         <v>0</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" ref="I9:I11" si="0">G9-H9</f>
+        <f t="shared" ref="I9:I11" si="1">G9-H9</f>
         <v>3333</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="145"/>
+      <c r="L9" s="113"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -3599,7 +3632,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J10" s="1"/>
@@ -3618,7 +3651,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J11" s="1"/>
@@ -3716,7 +3749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D33D141-6777-454F-A53F-584318966504}">
   <dimension ref="B1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -3746,52 +3779,52 @@
   <sheetData>
     <row r="1" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="147" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="147" t="s">
+      <c r="C2" s="115" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="147" t="s">
+      <c r="E2" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="147" t="s">
+      <c r="F2" s="115" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="147" t="s">
+      <c r="G2" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="147" t="s">
+      <c r="H2" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="147" t="s">
+      <c r="I2" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="147" t="s">
+      <c r="J2" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="147" t="s">
+      <c r="K2" s="115" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="147" t="s">
+      <c r="L2" s="115" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="147" t="s">
+      <c r="M2" s="115" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="147" t="s">
+      <c r="N2" s="115" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="147" t="s">
+      <c r="O2" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="147" t="s">
+      <c r="P2" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="148" t="s">
+      <c r="Q2" s="116" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3820,7 +3853,7 @@
       <c r="K3" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="149" t="s">
+      <c r="L3" s="117" t="s">
         <v>186</v>
       </c>
       <c r="M3" s="40" t="s">
@@ -3854,7 +3887,7 @@
       <c r="K4" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="149" t="s">
+      <c r="L4" s="117" t="s">
         <v>186</v>
       </c>
       <c r="M4" s="40" t="s">
@@ -3888,7 +3921,7 @@
       <c r="K5" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="149" t="s">
+      <c r="L5" s="117" t="s">
         <v>186</v>
       </c>
       <c r="M5" s="40" t="s">
@@ -3916,7 +3949,7 @@
         <f>H6</f>
         <v>9000</v>
       </c>
-      <c r="J6" s="150">
+      <c r="J6" s="118">
         <v>45299</v>
       </c>
       <c r="K6" s="40"/>
@@ -4062,14 +4095,14 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="114"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="121"/>
       <c r="M2" s="79" t="s">
         <v>111</v>
       </c>
@@ -4084,28 +4117,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="122" t="s">
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="131"/>
       <c r="M3" s="53"/>
       <c r="N3" s="34"/>
       <c r="O3" s="53"/>
       <c r="P3" s="34"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="127" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="9"/>
@@ -4128,8 +4161,8 @@
       <c r="P4" s="34"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="128"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -4296,10 +4329,10 @@
       <c r="P11" s="34"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="124"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -4605,16 +4638,16 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="119" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="114"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="121"/>
       <c r="O2" s="79" t="s">
         <v>111</v>
       </c>
@@ -4629,30 +4662,30 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="122" t="s">
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="124"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="131"/>
       <c r="O3" s="53"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="125" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="120" t="s">
+      <c r="C4" s="127" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="82"/>
@@ -4677,8 +4710,8 @@
       <c r="R4" s="34"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="128"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
@@ -4859,10 +4892,10 @@
       <c r="R11" s="34"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="126"/>
+      <c r="C12" s="133"/>
       <c r="D12" s="80"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -4967,19 +5000,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="137" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="133"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="140"/>
       <c r="Q2" s="55" t="s">
         <v>111</v>
       </c>
@@ -4994,30 +5027,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="123"/>
-      <c r="O3" s="124"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="131"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
       <c r="S3" s="53"/>
       <c r="T3" s="34"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="127" t="s">
+      <c r="B4" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="129" t="s">
+      <c r="C4" s="136" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="106">
@@ -5046,8 +5079,8 @@
       <c r="T4" s="78"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="128"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="135"/>
+      <c r="C5" s="128"/>
       <c r="D5" s="33" t="s">
         <v>167</v>
       </c>
@@ -5246,10 +5279,10 @@
       <c r="T11" s="78"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="124" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="124"/>
       <c r="D12" s="34" t="s">
         <v>168</v>
       </c>
@@ -5479,19 +5512,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="119" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="114"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="121"/>
       <c r="Q2" s="55" t="s">
         <v>111</v>
       </c>
@@ -5506,30 +5539,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="115"/>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="123"/>
-      <c r="O3" s="124"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="148"/>
+      <c r="M3" s="129"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="131"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
       <c r="S3" s="53"/>
       <c r="T3" s="34"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="146" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="82"/>
@@ -5556,8 +5589,8 @@
       <c r="T4" s="78"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="119"/>
-      <c r="C5" s="121"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="128"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
@@ -5754,10 +5787,10 @@
       <c r="T11" s="34"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="147" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="124"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>

</xml_diff>

<commit_message>
Ops Jan-2024 and Antech Docs
Ops Jan-2024 and Antech Docs
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550575C5-E1C7-425B-AD14-9CA10A6250FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="10" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -26,7 +25,7 @@
     <sheet name="B6" sheetId="11" r:id="rId11"/>
     <sheet name="B7" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,17 +44,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={9982AFAF-E6E7-45C0-A44A-0C0167B0574C}</author>
   </authors>
   <commentList>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{04A41BDB-6338-4F4D-A6D7-1E904B9507AF}">
+    <comment ref="D12" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     1) Redox</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -63,17 +71,26 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={E5C95DD1-C6DB-4079-AFA4-BCF3BDF94C7F}</author>
   </authors>
   <commentList>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E5C95DD1-C6DB-4079-AFA4-BCF3BDF94C7F}">
+    <comment ref="D12" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     An introduction to Management - Evolution, Concept, Definition, Features, Objectives, Scope</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -81,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="201">
   <si>
     <t>Course</t>
   </si>
@@ -679,16 +696,28 @@
   </si>
   <si>
     <t>B7</t>
+  </si>
+  <si>
+    <t>1) Mettalurgy</t>
+  </si>
+  <si>
+    <t>1) MCQ Practice</t>
+  </si>
+  <si>
+    <t>1) Probability &amp;</t>
+  </si>
+  <si>
+    <t>Revision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -774,12 +803,6 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1820,135 +1843,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1959,6 +1853,135 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2294,7 +2317,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C90D3B1-C76E-4CE0-A4AA-1FA923F6E3CF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2353,7 +2376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D3BDFFA-3B28-4FBD-9FBD-B0268E77162A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2376,14 +2399,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="138" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="169"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="175"/>
       <c r="M2" s="54" t="s">
         <v>113</v>
       </c>
@@ -2401,18 +2424,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="141" t="s">
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="143"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
+      <c r="K3" s="149"/>
       <c r="M3" s="34"/>
       <c r="N3" s="53"/>
       <c r="O3" s="34"/>
@@ -2420,10 +2443,10 @@
       <c r="Q3" s="34"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="145" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="9"/>
@@ -2449,8 +2472,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="138"/>
-      <c r="C5" s="140"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -2624,10 +2647,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="51"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -3066,10 +3089,10 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C94FC2-4E02-4E43-9E5D-811D6F46FE15}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
@@ -3086,19 +3109,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="157" t="s">
+      <c r="B2" s="163" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="174"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="179"/>
+      <c r="L2" s="180"/>
       <c r="N2" s="34"/>
       <c r="O2" s="108" t="s">
         <v>165</v>
@@ -3107,17 +3130,17 @@
       <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="176"/>
+      <c r="K3" s="176"/>
+      <c r="L3" s="176"/>
       <c r="N3" s="55" t="s">
         <v>111</v>
       </c>
@@ -3132,10 +3155,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="177" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="171" t="s">
+      <c r="C4" s="177" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="96">
@@ -3161,8 +3184,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="171"/>
-      <c r="C5" s="171"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
       <c r="D5" s="97" t="s">
         <v>163</v>
       </c>
@@ -3333,10 +3356,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="34" t="s">
         <v>164</v>
       </c>
@@ -3408,76 +3431,76 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="N15" s="175"/>
-      <c r="O15" s="176"/>
-      <c r="P15" s="175"/>
-      <c r="Q15" s="175"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="133"/>
+      <c r="P15" s="132"/>
+      <c r="Q15" s="132"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="177"/>
-      <c r="O16" s="176"/>
-      <c r="P16" s="177"/>
-      <c r="Q16" s="176"/>
+      <c r="N16" s="134"/>
+      <c r="O16" s="133"/>
+      <c r="P16" s="134"/>
+      <c r="Q16" s="133"/>
     </row>
     <row r="17" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N17" s="178"/>
-      <c r="O17" s="175"/>
-      <c r="P17" s="178"/>
-      <c r="Q17" s="175"/>
+      <c r="N17" s="135"/>
+      <c r="O17" s="132"/>
+      <c r="P17" s="135"/>
+      <c r="Q17" s="132"/>
     </row>
     <row r="18" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N18" s="178"/>
-      <c r="O18" s="175"/>
-      <c r="P18" s="178"/>
-      <c r="Q18" s="175"/>
+      <c r="N18" s="135"/>
+      <c r="O18" s="132"/>
+      <c r="P18" s="135"/>
+      <c r="Q18" s="132"/>
     </row>
     <row r="19" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N19" s="178"/>
-      <c r="O19" s="175"/>
-      <c r="P19" s="178"/>
-      <c r="Q19" s="175"/>
+      <c r="N19" s="135"/>
+      <c r="O19" s="132"/>
+      <c r="P19" s="135"/>
+      <c r="Q19" s="132"/>
     </row>
     <row r="20" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N20" s="178"/>
-      <c r="O20" s="175"/>
-      <c r="P20" s="178"/>
-      <c r="Q20" s="175"/>
+      <c r="N20" s="135"/>
+      <c r="O20" s="132"/>
+      <c r="P20" s="135"/>
+      <c r="Q20" s="132"/>
     </row>
     <row r="21" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N21" s="178"/>
-      <c r="O21" s="175"/>
-      <c r="P21" s="178"/>
-      <c r="Q21" s="175"/>
+      <c r="N21" s="135"/>
+      <c r="O21" s="132"/>
+      <c r="P21" s="135"/>
+      <c r="Q21" s="132"/>
     </row>
     <row r="22" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N22" s="178"/>
-      <c r="O22" s="175"/>
-      <c r="P22" s="178"/>
-      <c r="Q22" s="175"/>
+      <c r="N22" s="135"/>
+      <c r="O22" s="132"/>
+      <c r="P22" s="135"/>
+      <c r="Q22" s="132"/>
     </row>
     <row r="23" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N23" s="178"/>
-      <c r="O23" s="175"/>
-      <c r="P23" s="178"/>
-      <c r="Q23" s="175"/>
+      <c r="N23" s="135"/>
+      <c r="O23" s="132"/>
+      <c r="P23" s="135"/>
+      <c r="Q23" s="132"/>
     </row>
     <row r="24" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N24" s="178"/>
-      <c r="O24" s="176"/>
-      <c r="P24" s="177"/>
-      <c r="Q24" s="175"/>
+      <c r="N24" s="135"/>
+      <c r="O24" s="133"/>
+      <c r="P24" s="134"/>
+      <c r="Q24" s="132"/>
     </row>
     <row r="25" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N25" s="178"/>
-      <c r="O25" s="176"/>
-      <c r="P25" s="177"/>
-      <c r="Q25" s="175"/>
+      <c r="N25" s="135"/>
+      <c r="O25" s="133"/>
+      <c r="P25" s="134"/>
+      <c r="Q25" s="132"/>
     </row>
     <row r="26" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N26" s="178"/>
-      <c r="O26" s="176"/>
-      <c r="P26" s="177"/>
-      <c r="Q26" s="175"/>
+      <c r="N26" s="135"/>
+      <c r="O26" s="133"/>
+      <c r="P26" s="134"/>
+      <c r="Q26" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3493,7 +3516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849B863B-15B9-415C-AEAC-F7280787DF3E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3511,19 +3534,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="157" t="s">
+      <c r="B2" s="163" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="173"/>
-      <c r="L2" s="174"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
+      <c r="H2" s="163"/>
+      <c r="I2" s="163"/>
+      <c r="J2" s="178"/>
+      <c r="K2" s="179"/>
+      <c r="L2" s="180"/>
       <c r="N2" s="34"/>
       <c r="O2" s="108" t="s">
         <v>174</v>
@@ -3532,17 +3555,17 @@
       <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="170"/>
-      <c r="K3" s="170"/>
-      <c r="L3" s="170"/>
+      <c r="B3" s="163"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="176"/>
+      <c r="K3" s="176"/>
+      <c r="L3" s="176"/>
       <c r="N3" s="55" t="s">
         <v>111</v>
       </c>
@@ -3557,10 +3580,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="177" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="171" t="s">
+      <c r="C4" s="177" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="96">
@@ -3586,8 +3609,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="171"/>
-      <c r="C5" s="171"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
       <c r="D5" s="97" t="s">
         <v>163</v>
       </c>
@@ -3758,10 +3781,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -3829,19 +3852,19 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="N15" s="175"/>
-      <c r="O15" s="176"/>
-      <c r="P15" s="175"/>
-      <c r="Q15" s="175"/>
+      <c r="N15" s="132"/>
+      <c r="O15" s="133"/>
+      <c r="P15" s="132"/>
+      <c r="Q15" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B2:I3"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3849,7 +3872,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DF67B1-7A31-46BB-8007-D9F915FBEBAF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4161,18 +4184,18 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="179" t="s">
+      <c r="F13" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="180">
+      <c r="G13" s="137">
         <f>SUM(G3:G12)</f>
         <v>12000</v>
       </c>
-      <c r="H13" s="180">
+      <c r="H13" s="137">
         <f>SUM(H3:H12)</f>
         <v>12000</v>
       </c>
-      <c r="I13" s="180">
+      <c r="I13" s="137">
         <f>SUM(I3:I12)</f>
         <v>0</v>
       </c>
@@ -4183,7 +4206,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D33D141-6777-454F-A53F-584318966504}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:Q7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -4420,7 +4443,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1681C941-35C2-49C0-B4BB-FB590551761B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4434,7 +4457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC6DCCC-E30E-4525-A65D-DF43CA79E3C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -4509,7 +4532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45B9C15-B318-4180-B0D5-96F2E895A4B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4532,18 +4555,18 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="138" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="144"/>
-      <c r="I2" s="145"/>
-      <c r="J2" s="145"/>
-      <c r="K2" s="146"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="150"/>
+      <c r="I2" s="151"/>
+      <c r="J2" s="151"/>
+      <c r="K2" s="152"/>
       <c r="M2" s="76" t="s">
         <v>111</v>
       </c>
@@ -4558,28 +4581,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="141" t="s">
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="142"/>
-      <c r="J3" s="142"/>
-      <c r="K3" s="143"/>
+      <c r="I3" s="148"/>
+      <c r="J3" s="148"/>
+      <c r="K3" s="149"/>
       <c r="M3" s="53"/>
       <c r="N3" s="34"/>
       <c r="O3" s="53"/>
       <c r="P3" s="34"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="145" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="9"/>
@@ -4602,8 +4625,8 @@
       <c r="P4" s="34"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="138"/>
-      <c r="C5" s="140"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -4770,10 +4793,10 @@
       <c r="P11" s="34"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="142" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -5067,11 +5090,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5088,16 +5111,16 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="138" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
       <c r="J2" s="124"/>
       <c r="K2" s="125"/>
       <c r="L2" s="125"/>
@@ -5116,36 +5139,38 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="141" t="s">
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="142"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="143"/>
+      <c r="K3" s="148"/>
+      <c r="L3" s="148"/>
+      <c r="M3" s="149"/>
       <c r="O3" s="53"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="143" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="139" t="s">
+      <c r="C4" s="145" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="79">
         <v>45300</v>
       </c>
-      <c r="E4" s="79"/>
+      <c r="E4" s="79">
+        <v>45307</v>
+      </c>
       <c r="F4" s="79"/>
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>
@@ -5166,12 +5191,14 @@
       <c r="R4" s="34"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="138"/>
-      <c r="C5" s="140"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>185</v>
+      </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
@@ -5201,7 +5228,9 @@
       <c r="D6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -5227,7 +5256,7 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="14"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
@@ -5236,14 +5265,14 @@
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="15"/>
-      <c r="O7" s="53">
+      <c r="O7" s="74">
         <v>4</v>
       </c>
-      <c r="P7" s="34" t="s">
+      <c r="P7" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="Q7" s="53">
-        <v>0</v>
+      <c r="Q7" s="74">
+        <v>1</v>
       </c>
       <c r="R7" s="34"/>
     </row>
@@ -5253,7 +5282,7 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="14"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
@@ -5279,7 +5308,7 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
@@ -5288,14 +5317,14 @@
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="15"/>
-      <c r="O9" s="53">
+      <c r="O9" s="74">
         <v>6</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="P9" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="Q9" s="53">
-        <v>0</v>
+      <c r="Q9" s="74">
+        <v>1</v>
       </c>
       <c r="R9" s="34"/>
     </row>
@@ -5305,7 +5334,7 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="13"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="14"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -5331,7 +5360,7 @@
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="E11" s="16"/>
       <c r="F11" s="17"/>
       <c r="G11" s="65"/>
       <c r="H11" s="65"/>
@@ -5352,14 +5381,16 @@
       <c r="R11" s="34"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="153" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="148"/>
+      <c r="C12" s="154"/>
       <c r="D12" s="77" t="s">
         <v>186</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="34" t="s">
+        <v>197</v>
+      </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
@@ -5388,7 +5419,7 @@
       </c>
       <c r="Q13" s="76">
         <f>SUM(Q4:Q11)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R13" s="34"/>
     </row>
@@ -5422,7 +5453,7 @@
       </c>
       <c r="Q15" s="76">
         <f>ROUND((Q13/Q14)*100,2)</f>
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="R15" s="34"/>
     </row>
@@ -5443,11 +5474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5470,19 +5501,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="158" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="154"/>
-      <c r="J2" s="154"/>
-      <c r="K2" s="154"/>
-      <c r="L2" s="155"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="161"/>
       <c r="Q2" s="55" t="s">
         <v>111</v>
       </c>
@@ -5497,30 +5528,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="156"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="158"/>
-      <c r="J3" s="158"/>
-      <c r="K3" s="158"/>
-      <c r="L3" s="159"/>
-      <c r="M3" s="141"/>
-      <c r="N3" s="142"/>
-      <c r="O3" s="143"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="164"/>
+      <c r="J3" s="164"/>
+      <c r="K3" s="164"/>
+      <c r="L3" s="165"/>
+      <c r="M3" s="147"/>
+      <c r="N3" s="148"/>
+      <c r="O3" s="149"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
       <c r="S3" s="53"/>
       <c r="T3" s="34"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="149" t="s">
+      <c r="B4" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="157" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="103">
@@ -5529,7 +5560,9 @@
       <c r="E4" s="103">
         <v>45300</v>
       </c>
-      <c r="F4" s="103"/>
+      <c r="F4" s="103">
+        <v>45307</v>
+      </c>
       <c r="G4" s="103"/>
       <c r="H4" s="103"/>
       <c r="I4" s="96"/>
@@ -5551,15 +5584,17 @@
       <c r="T4" s="75"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="150"/>
-      <c r="C5" s="140"/>
+      <c r="B5" s="156"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="33" t="s">
         <v>166</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="33" t="s">
+        <v>187</v>
+      </c>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="97"/>
@@ -5593,7 +5628,9 @@
       <c r="E6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="14"/>
@@ -5755,17 +5792,19 @@
       <c r="T11" s="75"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="136" t="s">
+      <c r="B12" s="142" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="34" t="s">
         <v>167</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="34" t="s">
+        <v>198</v>
+      </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
@@ -5962,11 +6001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5990,22 +6029,22 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="138" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="133"/>
-      <c r="I2" s="133"/>
-      <c r="J2" s="133"/>
-      <c r="K2" s="133"/>
-      <c r="L2" s="133"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="167"/>
-      <c r="O2" s="168"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="139"/>
+      <c r="E2" s="139"/>
+      <c r="F2" s="139"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="172"/>
+      <c r="N2" s="173"/>
+      <c r="O2" s="174"/>
       <c r="Q2" s="55" t="s">
         <v>111</v>
       </c>
@@ -6020,36 +6059,38 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="160"/>
-      <c r="N3" s="161"/>
-      <c r="O3" s="162"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="166"/>
+      <c r="N3" s="167"/>
+      <c r="O3" s="168"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
       <c r="S3" s="53"/>
       <c r="T3" s="34"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="169" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="170" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="79">
         <v>45300</v>
       </c>
-      <c r="E4" s="79"/>
+      <c r="E4" s="79">
+        <v>45307</v>
+      </c>
       <c r="F4" s="79"/>
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>
@@ -6072,12 +6113,14 @@
       <c r="T4" s="75"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="138"/>
-      <c r="C5" s="140"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="33" t="s">
+        <v>189</v>
+      </c>
       <c r="F5" s="33"/>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
@@ -6109,7 +6152,9 @@
       <c r="D6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -6137,7 +6182,7 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="34"/>
-      <c r="E7" s="14"/>
+      <c r="E7" s="34"/>
       <c r="F7" s="14"/>
       <c r="G7" s="21"/>
       <c r="H7" s="34"/>
@@ -6167,7 +6212,7 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="34"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="34"/>
       <c r="F8" s="14"/>
       <c r="G8" s="21"/>
       <c r="H8" s="34"/>
@@ -6195,7 +6240,7 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="34"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="34"/>
       <c r="F9" s="14"/>
       <c r="G9" s="21"/>
       <c r="H9" s="34"/>
@@ -6223,7 +6268,7 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="34"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="34"/>
       <c r="F10" s="14"/>
       <c r="G10" s="21"/>
       <c r="H10" s="34"/>
@@ -6251,7 +6296,7 @@
       </c>
       <c r="C11" s="81"/>
       <c r="D11" s="84"/>
-      <c r="E11" s="83"/>
+      <c r="E11" s="84"/>
       <c r="F11" s="83"/>
       <c r="G11" s="35"/>
       <c r="H11" s="84"/>
@@ -6274,14 +6319,16 @@
       <c r="T11" s="34"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="165" t="s">
+      <c r="B12" s="171" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="136"/>
+      <c r="C12" s="142"/>
       <c r="D12" s="34" t="s">
         <v>190</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="34" t="s">
+        <v>199</v>
+      </c>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
@@ -6309,7 +6356,9 @@
       <c r="D13" s="34" t="s">
         <v>191</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="34" t="s">
+        <v>135</v>
+      </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
@@ -6335,7 +6384,9 @@
       <c r="B14" s="86"/>
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
+      <c r="E14" s="34" t="s">
+        <v>200</v>
+      </c>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>

</xml_diff>

<commit_message>
Ops done for Avishek
Ops done for Avishek
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9945673-5F9D-4AF8-BD7C-3D24F18B7A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="6"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -25,7 +26,7 @@
     <sheet name="B6" sheetId="11" r:id="rId11"/>
     <sheet name="B7" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,26 +45,17 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={9982AFAF-E6E7-45C0-A44A-0C0167B0574C}</author>
   </authors>
   <commentList>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     1) Redox</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -71,26 +63,17 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={E5C95DD1-C6DB-4079-AFA4-BCF3BDF94C7F}</author>
   </authors>
   <commentList>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     An introduction to Management - Evolution, Concept, Definition, Features, Objectives, Scope</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -98,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="204">
   <si>
     <t>Course</t>
   </si>
@@ -708,12 +691,21 @@
   </si>
   <si>
     <t>Revision</t>
+  </si>
+  <si>
+    <t>1) Mettalurgy - Doubt</t>
+  </si>
+  <si>
+    <t>Clearing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Probability </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
@@ -1550,7 +1542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1843,12 +1835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2317,7 +2304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2376,7 +2363,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="B1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2399,14 +2386,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="135" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="175"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="172"/>
       <c r="M2" s="54" t="s">
         <v>113</v>
       </c>
@@ -2424,18 +2411,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="147" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="149"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="145"/>
+      <c r="K3" s="146"/>
       <c r="M3" s="34"/>
       <c r="N3" s="53"/>
       <c r="O3" s="34"/>
@@ -2443,10 +2430,10 @@
       <c r="Q3" s="34"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="142" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="9"/>
@@ -2472,8 +2459,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="143"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -2647,10 +2634,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="51"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -3089,7 +3076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="B2:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3109,19 +3096,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="160" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="179"/>
-      <c r="L2" s="180"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="175"/>
+      <c r="K2" s="176"/>
+      <c r="L2" s="177"/>
       <c r="N2" s="34"/>
       <c r="O2" s="108" t="s">
         <v>165</v>
@@ -3130,17 +3117,17 @@
       <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="173"/>
+      <c r="K3" s="173"/>
+      <c r="L3" s="173"/>
       <c r="N3" s="55" t="s">
         <v>111</v>
       </c>
@@ -3155,10 +3142,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="174" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="174" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="96">
@@ -3184,8 +3171,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
+      <c r="B5" s="174"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="97" t="s">
         <v>163</v>
       </c>
@@ -3356,10 +3343,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="34" t="s">
         <v>164</v>
       </c>
@@ -3431,76 +3418,56 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="133"/>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="132"/>
+      <c r="O15" s="42"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="134"/>
-      <c r="O16" s="133"/>
-      <c r="P16" s="134"/>
-      <c r="Q16" s="133"/>
-    </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N17" s="135"/>
-      <c r="O17" s="132"/>
-      <c r="P17" s="135"/>
-      <c r="Q17" s="132"/>
-    </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N18" s="135"/>
-      <c r="O18" s="132"/>
-      <c r="P18" s="135"/>
-      <c r="Q18" s="132"/>
-    </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N19" s="135"/>
-      <c r="O19" s="132"/>
-      <c r="P19" s="135"/>
-      <c r="Q19" s="132"/>
-    </row>
-    <row r="20" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N20" s="135"/>
-      <c r="O20" s="132"/>
-      <c r="P20" s="135"/>
-      <c r="Q20" s="132"/>
-    </row>
-    <row r="21" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N21" s="135"/>
-      <c r="O21" s="132"/>
-      <c r="P21" s="135"/>
-      <c r="Q21" s="132"/>
-    </row>
-    <row r="22" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N22" s="135"/>
-      <c r="O22" s="132"/>
-      <c r="P22" s="135"/>
-      <c r="Q22" s="132"/>
-    </row>
-    <row r="23" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N23" s="135"/>
-      <c r="O23" s="132"/>
-      <c r="P23" s="135"/>
-      <c r="Q23" s="132"/>
-    </row>
-    <row r="24" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N24" s="135"/>
-      <c r="O24" s="133"/>
-      <c r="P24" s="134"/>
-      <c r="Q24" s="132"/>
-    </row>
-    <row r="25" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N25" s="135"/>
-      <c r="O25" s="133"/>
-      <c r="P25" s="134"/>
-      <c r="Q25" s="132"/>
-    </row>
-    <row r="26" spans="14:17" x14ac:dyDescent="0.3">
-      <c r="N26" s="135"/>
-      <c r="O26" s="133"/>
-      <c r="P26" s="134"/>
-      <c r="Q26" s="132"/>
+      <c r="N16" s="132"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="132"/>
+      <c r="Q16" s="42"/>
+    </row>
+    <row r="17" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N17" s="52"/>
+      <c r="P17" s="52"/>
+    </row>
+    <row r="18" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N18" s="52"/>
+      <c r="P18" s="52"/>
+    </row>
+    <row r="19" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N19" s="52"/>
+      <c r="P19" s="52"/>
+    </row>
+    <row r="20" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N20" s="52"/>
+      <c r="P20" s="52"/>
+    </row>
+    <row r="21" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N21" s="52"/>
+      <c r="P21" s="52"/>
+    </row>
+    <row r="22" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N22" s="52"/>
+      <c r="P22" s="52"/>
+    </row>
+    <row r="23" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N23" s="52"/>
+      <c r="P23" s="52"/>
+    </row>
+    <row r="24" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N24" s="52"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="132"/>
+    </row>
+    <row r="25" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N25" s="52"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="132"/>
+    </row>
+    <row r="26" spans="14:16" x14ac:dyDescent="0.3">
+      <c r="N26" s="52"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="132"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3516,7 +3483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="B2:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3534,19 +3501,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="163" t="s">
+      <c r="B2" s="160" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="163"/>
-      <c r="H2" s="163"/>
-      <c r="I2" s="163"/>
-      <c r="J2" s="178"/>
-      <c r="K2" s="179"/>
-      <c r="L2" s="180"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="175"/>
+      <c r="K2" s="176"/>
+      <c r="L2" s="177"/>
       <c r="N2" s="34"/>
       <c r="O2" s="108" t="s">
         <v>174</v>
@@ -3555,17 +3522,17 @@
       <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="163"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="163"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="160"/>
+      <c r="J3" s="173"/>
+      <c r="K3" s="173"/>
+      <c r="L3" s="173"/>
       <c r="N3" s="55" t="s">
         <v>111</v>
       </c>
@@ -3580,10 +3547,10 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="174" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="177" t="s">
+      <c r="C4" s="174" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="96">
@@ -3609,8 +3576,8 @@
       <c r="Q4" s="34"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="177"/>
-      <c r="C5" s="177"/>
+      <c r="B5" s="174"/>
+      <c r="C5" s="174"/>
       <c r="D5" s="97" t="s">
         <v>163</v>
       </c>
@@ -3781,10 +3748,10 @@
       <c r="Q11" s="34"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -3852,10 +3819,7 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
-      <c r="N15" s="132"/>
-      <c r="O15" s="133"/>
-      <c r="P15" s="132"/>
-      <c r="Q15" s="132"/>
+      <c r="O15" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3872,7 +3836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4184,18 +4148,18 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="136" t="s">
+      <c r="F13" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="137">
+      <c r="G13" s="134">
         <f>SUM(G3:G12)</f>
         <v>12000</v>
       </c>
-      <c r="H13" s="137">
+      <c r="H13" s="134">
         <f>SUM(H3:H12)</f>
         <v>12000</v>
       </c>
-      <c r="I13" s="137">
+      <c r="I13" s="134">
         <f>SUM(I3:I12)</f>
         <v>0</v>
       </c>
@@ -4206,7 +4170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:Q7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -4443,7 +4407,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4457,7 +4421,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
@@ -4532,7 +4496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4555,18 +4519,18 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="135" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="151"/>
-      <c r="J2" s="151"/>
-      <c r="K2" s="152"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="147"/>
+      <c r="I2" s="148"/>
+      <c r="J2" s="148"/>
+      <c r="K2" s="149"/>
       <c r="M2" s="76" t="s">
         <v>111</v>
       </c>
@@ -4581,28 +4545,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="147" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="149"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="145"/>
+      <c r="K3" s="146"/>
       <c r="M3" s="53"/>
       <c r="N3" s="34"/>
       <c r="O3" s="53"/>
       <c r="P3" s="34"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="142" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="9"/>
@@ -4625,8 +4589,8 @@
       <c r="P4" s="34"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="143"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
@@ -4793,10 +4757,10 @@
       <c r="P11" s="34"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -5090,11 +5054,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5111,16 +5075,16 @@
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="135" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
       <c r="J2" s="124"/>
       <c r="K2" s="125"/>
       <c r="L2" s="125"/>
@@ -5139,30 +5103,30 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="147" t="s">
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="144" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="148"/>
-      <c r="L3" s="148"/>
-      <c r="M3" s="149"/>
+      <c r="K3" s="145"/>
+      <c r="L3" s="145"/>
+      <c r="M3" s="146"/>
       <c r="O3" s="53"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="142" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="79">
@@ -5171,7 +5135,9 @@
       <c r="E4" s="79">
         <v>45307</v>
       </c>
-      <c r="F4" s="79"/>
+      <c r="F4" s="79">
+        <v>45309</v>
+      </c>
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>
       <c r="I4" s="116"/>
@@ -5191,15 +5157,17 @@
       <c r="R4" s="34"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="143"/>
       <c r="D5" s="33" t="s">
         <v>185</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="33" t="s">
+        <v>185</v>
+      </c>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="117"/>
@@ -5231,7 +5199,9 @@
       <c r="E6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="118"/>
@@ -5257,7 +5227,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
@@ -5283,7 +5253,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
@@ -5309,7 +5279,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="21"/>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
@@ -5335,7 +5305,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
@@ -5361,7 +5331,7 @@
       <c r="C11" s="8"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="65"/>
       <c r="H11" s="65"/>
       <c r="I11" s="66"/>
@@ -5381,17 +5351,19 @@
       <c r="R11" s="34"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="153" t="s">
+      <c r="B12" s="150" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="154"/>
+      <c r="C12" s="151"/>
       <c r="D12" s="77" t="s">
         <v>186</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>197</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="34" t="s">
+        <v>201</v>
+      </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
       <c r="I12" s="92"/>
@@ -5407,7 +5379,9 @@
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="F13" s="34" t="s">
+        <v>202</v>
+      </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
       <c r="I13" s="92"/>
@@ -5474,11 +5448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5488,7 +5462,8 @@
     <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="20.109375" customWidth="1"/>
     <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
@@ -5501,19 +5476,19 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="158" t="s">
+      <c r="B2" s="155" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="159"/>
-      <c r="D2" s="159"/>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
-      <c r="L2" s="161"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="157"/>
+      <c r="J2" s="157"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="158"/>
       <c r="Q2" s="55" t="s">
         <v>111</v>
       </c>
@@ -5528,30 +5503,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="162"/>
-      <c r="C3" s="163"/>
-      <c r="D3" s="163"/>
-      <c r="E3" s="163"/>
-      <c r="F3" s="163"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="163"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="164"/>
-      <c r="L3" s="165"/>
-      <c r="M3" s="147"/>
-      <c r="N3" s="148"/>
-      <c r="O3" s="149"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="160"/>
+      <c r="F3" s="160"/>
+      <c r="G3" s="160"/>
+      <c r="H3" s="160"/>
+      <c r="I3" s="161"/>
+      <c r="J3" s="161"/>
+      <c r="K3" s="161"/>
+      <c r="L3" s="162"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="145"/>
+      <c r="O3" s="146"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
       <c r="S3" s="53"/>
       <c r="T3" s="34"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="152" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="157" t="s">
+      <c r="C4" s="154" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="103">
@@ -5563,7 +5538,9 @@
       <c r="F4" s="103">
         <v>45307</v>
       </c>
-      <c r="G4" s="103"/>
+      <c r="G4" s="103">
+        <v>45309</v>
+      </c>
       <c r="H4" s="103"/>
       <c r="I4" s="96"/>
       <c r="J4" s="101"/>
@@ -5584,8 +5561,8 @@
       <c r="T4" s="75"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="156"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="143"/>
       <c r="D5" s="33" t="s">
         <v>166</v>
       </c>
@@ -5595,7 +5572,9 @@
       <c r="F5" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="G5" s="33"/>
+      <c r="G5" s="33" t="s">
+        <v>187</v>
+      </c>
       <c r="H5" s="33"/>
       <c r="I5" s="97"/>
       <c r="J5" s="102"/>
@@ -5631,7 +5610,9 @@
       <c r="F6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="H6" s="11"/>
       <c r="I6" s="14"/>
       <c r="J6" s="21"/>
@@ -5659,7 +5640,7 @@
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="21"/>
@@ -5687,7 +5668,7 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="21"/>
@@ -5715,7 +5696,7 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="21"/>
@@ -5743,7 +5724,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="21"/>
@@ -5792,10 +5773,10 @@
       <c r="T11" s="75"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="142" t="s">
+      <c r="B12" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="34" t="s">
         <v>167</v>
       </c>
@@ -5805,7 +5786,9 @@
       <c r="F12" s="34" t="s">
         <v>198</v>
       </c>
-      <c r="G12" s="34"/>
+      <c r="G12" s="34" t="s">
+        <v>167</v>
+      </c>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="92"/>
@@ -5814,16 +5797,16 @@
       <c r="M12" s="78"/>
       <c r="N12" s="34"/>
       <c r="O12" s="87"/>
-      <c r="Q12" s="53">
+      <c r="Q12" s="74">
         <v>9</v>
       </c>
-      <c r="R12" s="34" t="s">
+      <c r="R12" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="S12" s="53">
-        <v>0</v>
-      </c>
-      <c r="T12" s="34"/>
+      <c r="S12" s="74">
+        <v>1</v>
+      </c>
+      <c r="T12" s="75"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B13" s="34"/>
@@ -5958,7 +5941,7 @@
       </c>
       <c r="S21" s="76">
         <f>SUM(S4:S19)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="T21" s="34"/>
     </row>
@@ -5979,7 +5962,7 @@
       </c>
       <c r="S23" s="76">
         <f>ROUND((S21/S22)*100,2)</f>
-        <v>50</v>
+        <v>56.25</v>
       </c>
       <c r="T23" s="34"/>
     </row>
@@ -6001,11 +5984,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6029,22 +6012,22 @@
   <sheetData>
     <row r="1" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="135" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
-      <c r="H2" s="139"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="172"/>
-      <c r="N2" s="173"/>
-      <c r="O2" s="174"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="170"/>
+      <c r="O2" s="171"/>
       <c r="Q2" s="55" t="s">
         <v>111</v>
       </c>
@@ -6059,30 +6042,30 @@
       </c>
     </row>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="140"/>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="166"/>
-      <c r="N3" s="167"/>
-      <c r="O3" s="168"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="163"/>
+      <c r="N3" s="164"/>
+      <c r="O3" s="165"/>
       <c r="Q3" s="53"/>
       <c r="R3" s="34"/>
       <c r="S3" s="53"/>
       <c r="T3" s="34"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B4" s="169" t="s">
+      <c r="B4" s="166" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="170" t="s">
+      <c r="C4" s="167" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="79">
@@ -6091,7 +6074,9 @@
       <c r="E4" s="79">
         <v>45307</v>
       </c>
-      <c r="F4" s="79"/>
+      <c r="F4" s="79">
+        <v>45309</v>
+      </c>
       <c r="G4" s="79"/>
       <c r="H4" s="79"/>
       <c r="I4" s="79"/>
@@ -6113,15 +6098,17 @@
       <c r="T4" s="75"/>
     </row>
     <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="146"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="143"/>
       <c r="D5" s="33" t="s">
         <v>189</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>189</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="33" t="s">
+        <v>189</v>
+      </c>
       <c r="G5" s="33"/>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
@@ -6155,7 +6142,9 @@
       <c r="E6" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -6183,7 +6172,7 @@
       <c r="C7" s="6"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
-      <c r="F7" s="14"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="21"/>
       <c r="H7" s="34"/>
       <c r="I7" s="78"/>
@@ -6213,7 +6202,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
-      <c r="F8" s="14"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="21"/>
       <c r="H8" s="34"/>
       <c r="I8" s="78"/>
@@ -6241,7 +6230,7 @@
       <c r="C9" s="6"/>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
-      <c r="F9" s="14"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="21"/>
       <c r="H9" s="34"/>
       <c r="I9" s="78"/>
@@ -6269,7 +6258,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
-      <c r="F10" s="14"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="21"/>
       <c r="H10" s="34"/>
       <c r="I10" s="78"/>
@@ -6297,7 +6286,7 @@
       <c r="C11" s="81"/>
       <c r="D11" s="84"/>
       <c r="E11" s="84"/>
-      <c r="F11" s="83"/>
+      <c r="F11" s="84"/>
       <c r="G11" s="35"/>
       <c r="H11" s="84"/>
       <c r="I11" s="91"/>
@@ -6319,17 +6308,19 @@
       <c r="T11" s="34"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B12" s="171" t="s">
+      <c r="B12" s="168" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="142"/>
+      <c r="C12" s="139"/>
       <c r="D12" s="34" t="s">
         <v>190</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="34"/>
+      <c r="F12" s="34" t="s">
+        <v>203</v>
+      </c>
       <c r="G12" s="34"/>
       <c r="H12" s="34"/>
       <c r="I12" s="78"/>
@@ -6397,16 +6388,16 @@
       <c r="M14" s="86"/>
       <c r="N14" s="34"/>
       <c r="O14" s="6"/>
-      <c r="Q14" s="53">
+      <c r="Q14" s="74">
         <v>11</v>
       </c>
-      <c r="R14" s="34" t="s">
+      <c r="R14" s="75" t="s">
         <v>157</v>
       </c>
-      <c r="S14" s="53">
-        <v>0</v>
-      </c>
-      <c r="T14" s="34"/>
+      <c r="S14" s="74">
+        <v>1</v>
+      </c>
+      <c r="T14" s="75"/>
     </row>
     <row r="15" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="88"/>
@@ -6431,7 +6422,7 @@
       </c>
       <c r="S16" s="76">
         <f>SUM(S4:S14)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T16" s="34"/>
     </row>
@@ -6453,7 +6444,7 @@
       </c>
       <c r="S18" s="76">
         <f>ROUND((S16/S17)*100,2)</f>
-        <v>36.36</v>
+        <v>45.45</v>
       </c>
       <c r="T18" s="34"/>
     </row>

</xml_diff>

<commit_message>
Ops for Jan 2024 done
Ops for Jan 2024 done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9945673-5F9D-4AF8-BD7C-3D24F18B7A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3147EDA6-D975-41C6-8F80-1D2F1E2E44EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="208">
   <si>
     <t>Course</t>
   </si>
@@ -568,9 +568,6 @@
     <t>Oscillation</t>
   </si>
   <si>
-    <t>Straight Line finished</t>
-  </si>
-  <si>
     <t>Priyankshu Giri</t>
   </si>
   <si>
@@ -700,6 +697,21 @@
   </si>
   <si>
     <t xml:space="preserve">1) Probability </t>
+  </si>
+  <si>
+    <t>Slno</t>
+  </si>
+  <si>
+    <t>1) Mettalurgy &amp; Equilibrium</t>
+  </si>
+  <si>
+    <t>Doubt Clearing</t>
+  </si>
+  <si>
+    <t>1) Expansion of solids</t>
+  </si>
+  <si>
+    <t>1) Co-ordinate Geometry</t>
   </si>
 </sst>
 </file>
@@ -3097,7 +3109,7 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" s="160" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2" s="160"/>
       <c r="D2" s="160"/>
@@ -3111,7 +3123,7 @@
       <c r="L2" s="177"/>
       <c r="N2" s="34"/>
       <c r="O2" s="108" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P2" s="34"/>
       <c r="Q2" s="34"/>
@@ -3163,7 +3175,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P4" s="53">
         <v>0</v>
@@ -3174,7 +3186,7 @@
       <c r="B5" s="174"/>
       <c r="C5" s="174"/>
       <c r="D5" s="97" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" s="97"/>
       <c r="F5" s="97"/>
@@ -3188,7 +3200,7 @@
         <v>2</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P5" s="53">
         <v>0</v>
@@ -3200,10 +3212,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>162</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -3217,7 +3229,7 @@
         <v>3</v>
       </c>
       <c r="O6" s="34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="P6" s="53">
         <v>0</v>
@@ -3242,7 +3254,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P7" s="53">
         <v>0</v>
@@ -3267,7 +3279,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="34" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P8" s="53">
         <v>0</v>
@@ -3292,7 +3304,7 @@
         <v>6</v>
       </c>
       <c r="O9" s="34" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P9" s="53">
         <v>0</v>
@@ -3348,7 +3360,7 @@
       </c>
       <c r="C12" s="139"/>
       <c r="D12" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -3371,7 +3383,7 @@
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
@@ -3502,7 +3514,7 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" s="160" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C2" s="160"/>
       <c r="D2" s="160"/>
@@ -3516,7 +3528,7 @@
       <c r="L2" s="177"/>
       <c r="N2" s="34"/>
       <c r="O2" s="108" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P2" s="34"/>
       <c r="Q2" s="34"/>
@@ -3568,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P4" s="53">
         <v>0</v>
@@ -3579,7 +3591,7 @@
       <c r="B5" s="174"/>
       <c r="C5" s="174"/>
       <c r="D5" s="97" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E5" s="97"/>
       <c r="F5" s="97"/>
@@ -3593,7 +3605,7 @@
         <v>2</v>
       </c>
       <c r="O5" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P5" s="53">
         <v>0</v>
@@ -3605,10 +3617,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>161</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>162</v>
       </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
@@ -3622,7 +3634,7 @@
         <v>3</v>
       </c>
       <c r="O6" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P6" s="53">
         <v>0</v>
@@ -3647,7 +3659,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P7" s="53">
         <v>0</v>
@@ -3672,7 +3684,7 @@
         <v>5</v>
       </c>
       <c r="O8" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P8" s="53">
         <v>0</v>
@@ -3697,7 +3709,7 @@
         <v>6</v>
       </c>
       <c r="O9" s="34" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P9" s="53">
         <v>0</v>
@@ -4048,19 +4060,19 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G9" s="1">
         <v>1000</v>
@@ -4100,19 +4112,19 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G11" s="1">
         <v>1000</v>
@@ -4278,7 +4290,7 @@
         <v>44</v>
       </c>
       <c r="L3" s="114" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M3" s="40" t="s">
         <v>40</v>
@@ -4312,7 +4324,7 @@
         <v>44</v>
       </c>
       <c r="L4" s="114" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M4" s="40" t="s">
         <v>40</v>
@@ -4346,7 +4358,7 @@
         <v>44</v>
       </c>
       <c r="L5" s="114" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M5" s="40" t="s">
         <v>40</v>
@@ -5057,16 +5069,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:R16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
     <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="45.44140625" bestFit="1" customWidth="1"/>
@@ -5124,7 +5138,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="140" t="s">
-        <v>30</v>
+        <v>203</v>
       </c>
       <c r="C4" s="142" t="s">
         <v>27</v>
@@ -5138,7 +5152,9 @@
       <c r="F4" s="79">
         <v>45309</v>
       </c>
-      <c r="G4" s="79"/>
+      <c r="G4" s="79">
+        <v>45311</v>
+      </c>
       <c r="H4" s="79"/>
       <c r="I4" s="116"/>
       <c r="J4" s="27"/>
@@ -5160,15 +5176,17 @@
       <c r="B5" s="141"/>
       <c r="C5" s="143"/>
       <c r="D5" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="G5" s="33"/>
+        <v>184</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>184</v>
+      </c>
       <c r="H5" s="33"/>
       <c r="I5" s="117"/>
       <c r="J5" s="30"/>
@@ -5194,15 +5212,17 @@
         <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>161</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>161</v>
+      </c>
       <c r="H6" s="11"/>
       <c r="I6" s="118"/>
       <c r="J6" s="24"/>
@@ -5356,15 +5376,17 @@
       </c>
       <c r="C12" s="151"/>
       <c r="D12" s="77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="G12" s="34"/>
+        <v>200</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>204</v>
+      </c>
       <c r="H12" s="34"/>
       <c r="I12" s="92"/>
       <c r="J12" s="127"/>
@@ -5380,9 +5402,11 @@
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
       <c r="F13" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="G13" s="34"/>
+        <v>201</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>205</v>
+      </c>
       <c r="H13" s="34"/>
       <c r="I13" s="92"/>
       <c r="J13" s="127"/>
@@ -5451,8 +5475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:T24"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5460,8 +5484,7 @@
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.109375" bestFit="1" customWidth="1"/>
@@ -5541,7 +5564,9 @@
       <c r="G4" s="103">
         <v>45309</v>
       </c>
-      <c r="H4" s="103"/>
+      <c r="H4" s="103">
+        <v>45311</v>
+      </c>
       <c r="I4" s="96"/>
       <c r="J4" s="101"/>
       <c r="K4" s="96"/>
@@ -5564,18 +5589,20 @@
       <c r="B5" s="153"/>
       <c r="C5" s="143"/>
       <c r="D5" s="33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>187</v>
-      </c>
-      <c r="H5" s="33"/>
+        <v>186</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>186</v>
+      </c>
       <c r="I5" s="97"/>
       <c r="J5" s="102"/>
       <c r="K5" s="97"/>
@@ -5602,18 +5629,20 @@
         <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="H6" s="11"/>
+        <v>161</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>161</v>
+      </c>
       <c r="I6" s="14"/>
       <c r="J6" s="21"/>
       <c r="K6" s="14"/>
@@ -5778,18 +5807,20 @@
       </c>
       <c r="C12" s="139"/>
       <c r="D12" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="H12" s="34"/>
+        <v>166</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>206</v>
+      </c>
       <c r="I12" s="34"/>
       <c r="J12" s="92"/>
       <c r="K12" s="34"/>
@@ -5815,7 +5846,9 @@
       <c r="E13" s="34"/>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="34" t="s">
+        <v>205</v>
+      </c>
       <c r="I13" s="34"/>
       <c r="J13" s="92"/>
       <c r="K13" s="34"/>
@@ -5987,8 +6020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5998,7 +6031,7 @@
     <col min="4" max="4" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18.109375" customWidth="1"/>
     <col min="11" max="12" width="21.77734375" bestFit="1" customWidth="1"/>
@@ -6077,7 +6110,9 @@
       <c r="F4" s="79">
         <v>45309</v>
       </c>
-      <c r="G4" s="79"/>
+      <c r="G4" s="79">
+        <v>45311</v>
+      </c>
       <c r="H4" s="79"/>
       <c r="I4" s="79"/>
       <c r="J4" s="79"/>
@@ -6101,15 +6136,17 @@
       <c r="B5" s="141"/>
       <c r="C5" s="143"/>
       <c r="D5" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>189</v>
-      </c>
-      <c r="G5" s="33"/>
+        <v>188</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>188</v>
+      </c>
       <c r="H5" s="33"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
@@ -6137,15 +6174,17 @@
         <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="G6" s="11"/>
+        <v>161</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>161</v>
+      </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -6182,18 +6221,16 @@
       <c r="M7" s="22"/>
       <c r="N7" s="14"/>
       <c r="O7" s="15"/>
-      <c r="Q7" s="53">
+      <c r="Q7" s="75">
         <v>4</v>
       </c>
-      <c r="R7" s="34" t="s">
+      <c r="R7" s="75" t="s">
         <v>136</v>
       </c>
-      <c r="S7" s="53">
-        <v>0</v>
-      </c>
-      <c r="T7" s="34" t="s">
-        <v>160</v>
-      </c>
+      <c r="S7" s="74">
+        <v>1</v>
+      </c>
+      <c r="T7" s="75"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="5">
@@ -6313,15 +6350,17 @@
       </c>
       <c r="C12" s="139"/>
       <c r="D12" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="G12" s="34"/>
+        <v>202</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>207</v>
+      </c>
       <c r="H12" s="34"/>
       <c r="I12" s="78"/>
       <c r="J12" s="78"/>
@@ -6345,7 +6384,7 @@
       <c r="B13" s="86"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>135</v>
@@ -6376,7 +6415,7 @@
       <c r="C14" s="34"/>
       <c r="D14" s="34"/>
       <c r="E14" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
@@ -6422,7 +6461,7 @@
       </c>
       <c r="S16" s="76">
         <f>SUM(S4:S14)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T16" s="34"/>
     </row>
@@ -6444,7 +6483,7 @@
       </c>
       <c r="S18" s="76">
         <f>ROUND((S16/S17)*100,2)</f>
-        <v>45.45</v>
+        <v>54.55</v>
       </c>
       <c r="T18" s="34"/>
     </row>

</xml_diff>

<commit_message>
Updated Ops for Jan -2024
Updated Ops for Jan -2024
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2024/Ops-2024-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\Ops-2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCD979A-E5C7-4182-B597-55972622397C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20805877-F627-4C34-88A5-30ABEF7B7D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="577" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="229">
   <si>
     <t>Course</t>
   </si>
@@ -760,6 +760,21 @@
   </si>
   <si>
     <t>2) Complex Number</t>
+  </si>
+  <si>
+    <t>1) Monthly Class Test</t>
+  </si>
+  <si>
+    <t>Maths class did not</t>
+  </si>
+  <si>
+    <t xml:space="preserve">happen because she </t>
+  </si>
+  <si>
+    <t>and Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gave test on Physics  </t>
   </si>
 </sst>
 </file>
@@ -937,7 +952,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1399,17 +1414,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -1464,17 +1468,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1580,11 +1573,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1760,7 +1762,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1801,15 +1802,6 @@
     <xf numFmtId="14" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1839,7 +1831,7 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1847,12 +1839,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1895,15 +1886,15 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1913,7 +1904,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1937,33 +1928,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1976,12 +1958,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="5" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2399,14 +2401,14 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="121" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="161"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="153"/>
       <c r="M2" s="52" t="s">
         <v>113</v>
       </c>
@@ -2424,18 +2426,18 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="128"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="135" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="132"/>
       <c r="M3" s="32"/>
       <c r="N3" s="51"/>
       <c r="O3" s="32"/>
@@ -2443,10 +2445,10 @@
       <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="128" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="8"/>
@@ -2472,8 +2474,8 @@
       <c r="Q4" s="32"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="132"/>
-      <c r="C5" s="134"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="129"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
@@ -2647,10 +2649,10 @@
       <c r="Q11" s="32"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="49"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
@@ -3109,38 +3111,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="145" t="s">
         <v>191</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="166"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="158"/>
       <c r="N2" s="32"/>
-      <c r="O2" s="104" t="s">
+      <c r="O2" s="100" t="s">
         <v>164</v>
       </c>
       <c r="P2" s="32"/>
       <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
       <c r="N3" s="53" t="s">
         <v>111</v>
       </c>
@@ -3155,23 +3157,23 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="94">
+      <c r="D4" s="93">
         <v>45293</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
       <c r="N4" s="51">
         <v>1</v>
       </c>
@@ -3184,19 +3186,19 @@
       <c r="Q4" s="32"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="95" t="s">
+      <c r="B5" s="155"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="94" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
       <c r="N5" s="51">
         <v>2</v>
       </c>
@@ -3356,10 +3358,10 @@
       <c r="Q11" s="32"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="32" t="s">
         <v>163</v>
       </c>
@@ -3370,7 +3372,7 @@
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
-      <c r="L12" s="103"/>
+      <c r="L12" s="99"/>
       <c r="N12" s="51"/>
       <c r="O12" s="34" t="s">
         <v>116</v>
@@ -3434,9 +3436,9 @@
       <c r="O15" s="40"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="N16" s="122"/>
+      <c r="N16" s="117"/>
       <c r="O16" s="40"/>
-      <c r="P16" s="122"/>
+      <c r="P16" s="117"/>
       <c r="Q16" s="40"/>
     </row>
     <row r="17" spans="14:16" x14ac:dyDescent="0.3">
@@ -3470,17 +3472,17 @@
     <row r="24" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N24" s="50"/>
       <c r="O24" s="40"/>
-      <c r="P24" s="122"/>
+      <c r="P24" s="117"/>
     </row>
     <row r="25" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N25" s="50"/>
       <c r="O25" s="40"/>
-      <c r="P25" s="122"/>
+      <c r="P25" s="117"/>
     </row>
     <row r="26" spans="14:16" x14ac:dyDescent="0.3">
       <c r="N26" s="50"/>
       <c r="O26" s="40"/>
-      <c r="P26" s="122"/>
+      <c r="P26" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3514,38 +3516,38 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="150" t="s">
+      <c r="B2" s="145" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
-      <c r="H2" s="150"/>
-      <c r="I2" s="150"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="166"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
+      <c r="I2" s="145"/>
+      <c r="J2" s="156"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="158"/>
       <c r="N2" s="32"/>
-      <c r="O2" s="104" t="s">
+      <c r="O2" s="100" t="s">
         <v>173</v>
       </c>
       <c r="P2" s="32"/>
       <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="150"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="150"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
-      <c r="L3" s="162"/>
+      <c r="B3" s="145"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="154"/>
+      <c r="L3" s="154"/>
       <c r="N3" s="53" t="s">
         <v>111</v>
       </c>
@@ -3560,23 +3562,23 @@
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="155" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="155" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="94">
+      <c r="D4" s="93">
         <v>45299</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
+      <c r="H4" s="93"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
       <c r="N4" s="51">
         <v>1</v>
       </c>
@@ -3589,19 +3591,19 @@
       <c r="Q4" s="32"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="163"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="95" t="s">
+      <c r="B5" s="155"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="94" t="s">
         <v>162</v>
       </c>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
       <c r="N5" s="51">
         <v>2</v>
       </c>
@@ -3761,10 +3763,10 @@
       <c r="Q11" s="32"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
@@ -3773,7 +3775,7 @@
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
-      <c r="L12" s="103"/>
+      <c r="L12" s="99"/>
       <c r="N12" s="51"/>
       <c r="O12" s="34" t="s">
         <v>116</v>
@@ -3872,40 +3874,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="105" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="105" t="s">
+      <c r="C2" s="101" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="105" t="s">
+      <c r="E2" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="105" t="s">
+      <c r="F2" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="105" t="s">
+      <c r="G2" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="101" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="105" t="s">
+      <c r="I2" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="105" t="s">
+      <c r="J2" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="105" t="s">
+      <c r="K2" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="105" t="s">
+      <c r="M2" s="101" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3937,7 +3939,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="106">
+      <c r="L3" s="102">
         <v>45302</v>
       </c>
       <c r="M3" s="1" t="s">
@@ -3986,7 +3988,7 @@
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="106">
+      <c r="L5" s="102">
         <v>45302</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -4035,7 +4037,7 @@
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="106">
+      <c r="L7" s="102">
         <v>45302</v>
       </c>
       <c r="M7" s="1" t="s">
@@ -4087,7 +4089,7 @@
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="106">
+      <c r="L9" s="102">
         <v>45299</v>
       </c>
       <c r="M9" s="1" t="s">
@@ -4139,7 +4141,7 @@
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="106">
+      <c r="L11" s="102">
         <v>45299</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -4161,18 +4163,18 @@
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F13" s="123" t="s">
+      <c r="F13" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="124">
+      <c r="G13" s="119">
         <f>SUM(G3:G12)</f>
         <v>12000</v>
       </c>
-      <c r="H13" s="124">
+      <c r="H13" s="119">
         <f>SUM(H3:H12)</f>
         <v>12000</v>
       </c>
-      <c r="I13" s="124">
+      <c r="I13" s="119">
         <f>SUM(I3:I12)</f>
         <v>0</v>
       </c>
@@ -4216,52 +4218,52 @@
   <sheetData>
     <row r="1" spans="2:17" ht="12.6" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="108" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="108" t="s">
+      <c r="C2" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="108" t="s">
+      <c r="E2" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="108" t="s">
+      <c r="F2" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="108" t="s">
+      <c r="I2" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="108" t="s">
+      <c r="J2" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="108" t="s">
+      <c r="K2" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="108" t="s">
+      <c r="L2" s="104" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="108" t="s">
+      <c r="M2" s="104" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="108" t="s">
+      <c r="N2" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="108" t="s">
+      <c r="O2" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="108" t="s">
+      <c r="P2" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="109" t="s">
+      <c r="Q2" s="105" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4290,7 +4292,7 @@
       <c r="K3" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="110" t="s">
+      <c r="L3" s="106" t="s">
         <v>183</v>
       </c>
       <c r="M3" s="38" t="s">
@@ -4324,7 +4326,7 @@
       <c r="K4" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="110" t="s">
+      <c r="L4" s="106" t="s">
         <v>183</v>
       </c>
       <c r="M4" s="38" t="s">
@@ -4358,7 +4360,7 @@
       <c r="K5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="110" t="s">
+      <c r="L5" s="106" t="s">
         <v>183</v>
       </c>
       <c r="M5" s="38" t="s">
@@ -4386,7 +4388,7 @@
         <f>H6</f>
         <v>9000</v>
       </c>
-      <c r="J6" s="111">
+      <c r="J6" s="107">
         <v>45299</v>
       </c>
       <c r="K6" s="38"/>
@@ -4532,18 +4534,18 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="121" t="s">
         <v>120</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="140"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="133"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="135"/>
       <c r="M2" s="74" t="s">
         <v>111</v>
       </c>
@@ -4558,28 +4560,28 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="128"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="135" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
-      <c r="K3" s="137"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="132"/>
       <c r="M3" s="51"/>
       <c r="N3" s="32"/>
       <c r="O3" s="51"/>
       <c r="P3" s="32"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="128" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="8"/>
@@ -4602,12 +4604,12 @@
       <c r="P4" s="32"/>
     </row>
     <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="132"/>
-      <c r="C5" s="134"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="129"/>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
-      <c r="G5" s="112"/>
+      <c r="G5" s="108"/>
       <c r="H5" s="28"/>
       <c r="I5" s="29"/>
       <c r="J5" s="29"/>
@@ -4633,7 +4635,7 @@
       <c r="D6" s="10"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="113"/>
+      <c r="G6" s="109"/>
       <c r="H6" s="22"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23"/>
@@ -4770,16 +4772,16 @@
       <c r="P11" s="32"/>
     </row>
     <row r="12" spans="2:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="90"/>
-      <c r="H12" s="117"/>
-      <c r="K12" s="118"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="112"/>
+      <c r="K12" s="113"/>
       <c r="M12" s="72">
         <v>9</v>
       </c>
@@ -4797,9 +4799,9 @@
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="90"/>
-      <c r="H13" s="117"/>
-      <c r="K13" s="118"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="112"/>
+      <c r="K13" s="113"/>
       <c r="M13" s="51">
         <v>10</v>
       </c>
@@ -4817,11 +4819,11 @@
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="90"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="120"/>
-      <c r="J14" s="120"/>
-      <c r="K14" s="121"/>
+      <c r="G14" s="89"/>
+      <c r="H14" s="114"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="116"/>
       <c r="M14" s="51">
         <v>11</v>
       </c>
@@ -5071,7 +5073,7 @@
   <dimension ref="B1:R16"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:I14"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5082,7 +5084,9 @@
     <col min="5" max="6" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
     <col min="15" max="15" width="4.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="34.109375" customWidth="1"/>
@@ -5090,21 +5094,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="126" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="116"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
       <c r="O2" s="74" t="s">
         <v>111</v>
       </c>
@@ -5119,54 +5123,62 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="128"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="135" t="s">
+      <c r="B3" s="123"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="165" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="136"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="137"/>
+      <c r="L3" s="165"/>
+      <c r="M3" s="165"/>
       <c r="O3" s="51"/>
       <c r="P3" s="32"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="32"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="126" t="s">
         <v>203</v>
       </c>
-      <c r="C4" s="133" t="s">
+      <c r="C4" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="76">
         <v>45300</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="76">
         <v>45307</v>
       </c>
-      <c r="F4" s="77">
+      <c r="F4" s="76">
         <v>45309</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="76">
         <v>45311</v>
       </c>
-      <c r="H4" s="77">
+      <c r="H4" s="76">
         <v>45314</v>
       </c>
-      <c r="I4" s="77">
+      <c r="I4" s="162">
         <v>45318</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="27"/>
+      <c r="J4" s="93">
+        <v>45318</v>
+      </c>
+      <c r="K4" s="97" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="97" t="s">
+        <v>218</v>
+      </c>
+      <c r="M4" s="97" t="s">
+        <v>219</v>
+      </c>
       <c r="O4" s="51">
         <v>1</v>
       </c>
@@ -5179,8 +5191,8 @@
       <c r="R4" s="32"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="132"/>
-      <c r="C5" s="134"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="129"/>
       <c r="D5" s="31" t="s">
         <v>184</v>
       </c>
@@ -5196,13 +5208,15 @@
       <c r="H5" s="31" t="s">
         <v>184</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="163" t="s">
         <v>184</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="30"/>
+      <c r="J5" s="94" t="s">
+        <v>184</v>
+      </c>
+      <c r="K5" s="98"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
       <c r="O5" s="72">
         <v>2</v>
       </c>
@@ -5236,13 +5250,22 @@
       <c r="H6" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="164" t="s">
         <v>161</v>
       </c>
-      <c r="J6" s="22"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
+      <c r="J6" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="K6" s="13">
+        <v>72</v>
+      </c>
+      <c r="L6" s="13">
+        <v>48</v>
+      </c>
+      <c r="M6" s="13">
+        <f>ROUND((L6/K6)*100,2)</f>
+        <v>66.67</v>
+      </c>
       <c r="O6" s="51">
         <v>3</v>
       </c>
@@ -5265,10 +5288,10 @@
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
-      <c r="J7" s="20"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="M7" s="13"/>
       <c r="O7" s="72">
         <v>4</v>
       </c>
@@ -5291,10 +5314,10 @@
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
-      <c r="J8" s="20"/>
+      <c r="J8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
+      <c r="M8" s="13"/>
       <c r="O8" s="72">
         <v>5</v>
       </c>
@@ -5317,10 +5340,10 @@
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
-      <c r="J9" s="20"/>
+      <c r="J9" s="13"/>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
+      <c r="M9" s="13"/>
       <c r="O9" s="72">
         <v>6</v>
       </c>
@@ -5343,10 +5366,10 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="19"/>
-      <c r="J10" s="20"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
+      <c r="M10" s="13"/>
       <c r="O10" s="51">
         <v>7</v>
       </c>
@@ -5359,20 +5382,20 @@
       <c r="R10" s="32"/>
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="78">
+      <c r="B11" s="77">
         <v>6</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
       <c r="G11" s="68"/>
       <c r="H11" s="68"/>
       <c r="I11" s="69"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="16"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
       <c r="O11" s="51">
         <v>8</v>
       </c>
@@ -5385,40 +5408,50 @@
       <c r="R11" s="32"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="141" t="s">
+      <c r="B12" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="142"/>
-      <c r="D12" s="75" t="s">
+      <c r="C12" s="137"/>
+      <c r="D12" s="111" t="s">
         <v>185</v>
       </c>
-      <c r="E12" s="125" t="s">
+      <c r="E12" s="167" t="s">
         <v>196</v>
       </c>
-      <c r="F12" s="125" t="s">
+      <c r="F12" s="120" t="s">
         <v>200</v>
       </c>
-      <c r="G12" s="125" t="s">
+      <c r="G12" s="120" t="s">
         <v>204</v>
       </c>
-      <c r="H12" s="125" t="s">
+      <c r="H12" s="120" t="s">
         <v>210</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="159" t="s">
         <v>212</v>
       </c>
-      <c r="J12" s="117"/>
-      <c r="M12" s="118"/>
+      <c r="J12" s="120" t="s">
+        <v>224</v>
+      </c>
+      <c r="K12" s="120" t="s">
+        <v>220</v>
+      </c>
+      <c r="L12" s="120" t="s">
+        <v>221</v>
+      </c>
+      <c r="M12" s="168">
+        <v>45321</v>
+      </c>
       <c r="O12" s="51"/>
       <c r="P12" s="32"/>
       <c r="Q12" s="51"/>
       <c r="R12" s="32"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="84"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
+      <c r="D13" s="89"/>
+      <c r="E13" s="83"/>
       <c r="F13" s="32" t="s">
         <v>201</v>
       </c>
@@ -5428,11 +5461,13 @@
       <c r="H13" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="89" t="s">
         <v>213</v>
       </c>
-      <c r="J13" s="117"/>
-      <c r="M13" s="118"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="6"/>
       <c r="O13" s="51"/>
       <c r="P13" s="34" t="s">
         <v>122</v>
@@ -5444,20 +5479,20 @@
       <c r="R13" s="32"/>
     </row>
     <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="86"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="87"/>
-      <c r="G14" s="87"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="7" t="s">
+      <c r="B14" s="85"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="160"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="160" t="s">
         <v>214</v>
       </c>
-      <c r="J14" s="119"/>
-      <c r="K14" s="120"/>
-      <c r="L14" s="120"/>
-      <c r="M14" s="121"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="7"/>
       <c r="O14" s="51"/>
       <c r="P14" s="34" t="s">
         <v>116</v>
@@ -5469,6 +5504,9 @@
       <c r="R14" s="32"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="K15" s="161"/>
+      <c r="L15" s="161"/>
+      <c r="M15" s="161"/>
       <c r="O15" s="51"/>
       <c r="P15" s="34" t="s">
         <v>131</v>
@@ -5484,9 +5522,8 @@
       <c r="Q16" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B2:I3"/>
-    <mergeCell ref="J3:M3"/>
+  <mergeCells count="4">
+    <mergeCell ref="B2:J3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
@@ -5499,8 +5536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5524,18 +5561,18 @@
   <sheetData>
     <row r="1" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="141" t="s">
         <v>119</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="K2" s="148"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="143"/>
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
       <c r="P2" s="53" t="s">
         <v>111</v>
       </c>
@@ -5550,56 +5587,58 @@
       </c>
     </row>
     <row r="3" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="149"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="150"/>
-      <c r="E3" s="150"/>
-      <c r="F3" s="150"/>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
-      <c r="K3" s="151"/>
-      <c r="L3" s="135" t="s">
+      <c r="B3" s="144"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="145"/>
+      <c r="E3" s="145"/>
+      <c r="F3" s="145"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="136"/>
-      <c r="N3" s="137"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="132"/>
       <c r="P3" s="51"/>
       <c r="Q3" s="32"/>
       <c r="R3" s="51"/>
       <c r="S3" s="32"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="143" t="s">
+      <c r="B4" s="138" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="145" t="s">
+      <c r="C4" s="140" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="99">
+      <c r="D4" s="95">
         <v>45297</v>
       </c>
-      <c r="E4" s="99">
+      <c r="E4" s="95">
         <v>45300</v>
       </c>
-      <c r="F4" s="99">
+      <c r="F4" s="95">
         <v>45307</v>
       </c>
-      <c r="G4" s="99">
+      <c r="G4" s="95">
         <v>45309</v>
       </c>
-      <c r="H4" s="99">
+      <c r="H4" s="95">
         <v>45311</v>
       </c>
-      <c r="I4" s="99">
+      <c r="I4" s="95">
         <v>45314</v>
       </c>
-      <c r="J4" s="99">
+      <c r="J4" s="95">
         <v>45318</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="91" t="s">
+      <c r="K4" s="95">
+        <v>45321</v>
+      </c>
+      <c r="L4" s="90" t="s">
         <v>217</v>
       </c>
       <c r="M4" s="70" t="s">
@@ -5620,8 +5659,8 @@
       <c r="S4" s="73"/>
     </row>
     <row r="5" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="144"/>
-      <c r="C5" s="134"/>
+      <c r="B5" s="139"/>
+      <c r="C5" s="129"/>
       <c r="D5" s="31" t="s">
         <v>165</v>
       </c>
@@ -5643,8 +5682,10 @@
       <c r="J5" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="K5" s="95"/>
-      <c r="L5" s="92"/>
+      <c r="K5" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="L5" s="91"/>
       <c r="M5" s="29"/>
       <c r="N5" s="30"/>
       <c r="P5" s="72">
@@ -5659,7 +5700,7 @@
       <c r="S5" s="73"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="100">
+      <c r="B6" s="96">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -5686,16 +5727,18 @@
       <c r="J6" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="93">
-        <v>100</v>
+      <c r="K6" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="92">
+        <v>98</v>
       </c>
       <c r="M6" s="23">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N6" s="24">
         <f>ROUND((M6/L6)*100,2)</f>
-        <v>49</v>
+        <v>48.98</v>
       </c>
       <c r="P6" s="72">
         <v>3</v>
@@ -5816,22 +5859,22 @@
       </c>
       <c r="S10" s="73"/>
     </row>
-    <row r="11" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B11" s="51">
         <v>6</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="80"/>
-      <c r="M11" s="81"/>
-      <c r="N11" s="83"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="82"/>
       <c r="P11" s="72">
         <v>8</v>
       </c>
@@ -5844,10 +5887,10 @@
       <c r="S11" s="73"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="130" t="s">
+      <c r="B12" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="32" t="s">
         <v>166</v>
       </c>
@@ -5866,18 +5909,20 @@
       <c r="I12" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="K12" s="32"/>
-      <c r="L12" s="76" t="s">
+      <c r="K12" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="L12" s="32" t="s">
         <v>220</v>
       </c>
       <c r="M12" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="N12" s="85">
-        <v>45318</v>
+      <c r="N12" s="99">
+        <v>45321</v>
       </c>
       <c r="P12" s="72">
         <v>9</v>
@@ -5903,15 +5948,13 @@
       <c r="I13" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="32" t="s">
         <v>213</v>
       </c>
       <c r="K13" s="32"/>
-      <c r="L13" s="76" t="s">
-        <v>222</v>
-      </c>
+      <c r="L13" s="32"/>
       <c r="M13" s="32"/>
-      <c r="N13" s="6"/>
+      <c r="N13" s="32"/>
       <c r="P13" s="51">
         <v>10</v>
       </c>
@@ -5923,7 +5966,7 @@
       </c>
       <c r="S13" s="32"/>
     </row>
-    <row r="14" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
@@ -5931,16 +5974,14 @@
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
-      <c r="I14" s="90"/>
-      <c r="J14" s="7" t="s">
+      <c r="I14" s="32"/>
+      <c r="J14" s="32" t="s">
         <v>214</v>
       </c>
       <c r="K14" s="32"/>
-      <c r="L14" s="76" t="s">
-        <v>223</v>
-      </c>
+      <c r="L14" s="32"/>
       <c r="M14" s="32"/>
-      <c r="N14" s="6"/>
+      <c r="N14" s="32"/>
       <c r="P14" s="72">
         <v>11</v>
       </c>
@@ -5952,7 +5993,7 @@
       </c>
       <c r="S14" s="73"/>
     </row>
-    <row r="15" spans="2:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
       <c r="D15" s="32"/>
@@ -5960,12 +6001,12 @@
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
       <c r="K15" s="32"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="7"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
       <c r="P15" s="51">
         <v>12</v>
       </c>
@@ -6078,8 +6119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:R18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6101,21 +6142,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="126" t="s">
+    <row r="2" spans="2:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="121" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="127"/>
-      <c r="G2" s="127"/>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
-      <c r="J2" s="127"/>
-      <c r="K2" s="158"/>
-      <c r="L2" s="159"/>
-      <c r="M2" s="160"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="122"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="122"/>
+      <c r="K2" s="150"/>
+      <c r="L2" s="151"/>
+      <c r="M2" s="152"/>
       <c r="O2" s="53" t="s">
         <v>111</v>
       </c>
@@ -6130,52 +6171,62 @@
       </c>
     </row>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="128"/>
-      <c r="C3" s="129"/>
-      <c r="D3" s="129"/>
-      <c r="E3" s="129"/>
-      <c r="F3" s="129"/>
-      <c r="G3" s="129"/>
-      <c r="H3" s="129"/>
-      <c r="I3" s="129"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="152"/>
-      <c r="L3" s="153"/>
-      <c r="M3" s="154"/>
+      <c r="B3" s="123"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="130" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="131"/>
+      <c r="M3" s="132"/>
       <c r="O3" s="51"/>
       <c r="P3" s="32"/>
       <c r="Q3" s="51"/>
       <c r="R3" s="32"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="77">
+      <c r="D4" s="76">
         <v>45300</v>
       </c>
-      <c r="E4" s="77">
+      <c r="E4" s="76">
         <v>45307</v>
       </c>
-      <c r="F4" s="77">
+      <c r="F4" s="76">
         <v>45309</v>
       </c>
-      <c r="G4" s="77">
+      <c r="G4" s="76">
         <v>45311</v>
       </c>
-      <c r="H4" s="77">
+      <c r="H4" s="76">
         <v>45314</v>
       </c>
-      <c r="I4" s="77">
+      <c r="I4" s="76">
         <v>45318</v>
       </c>
-      <c r="J4" s="77"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="71"/>
+      <c r="J4" s="76">
+        <v>45321</v>
+      </c>
+      <c r="K4" s="90" t="s">
+        <v>217</v>
+      </c>
+      <c r="L4" s="70" t="s">
+        <v>218</v>
+      </c>
+      <c r="M4" s="71" t="s">
+        <v>219</v>
+      </c>
       <c r="O4" s="72">
         <v>1</v>
       </c>
@@ -6188,8 +6239,8 @@
       <c r="R4" s="73"/>
     </row>
     <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="132"/>
-      <c r="C5" s="134"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="129"/>
       <c r="D5" s="31" t="s">
         <v>188</v>
       </c>
@@ -6208,8 +6259,10 @@
       <c r="I5" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="J5" s="31"/>
-      <c r="K5" s="97"/>
+      <c r="J5" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="K5" s="91"/>
       <c r="L5" s="29"/>
       <c r="M5" s="30"/>
       <c r="O5" s="72">
@@ -6248,10 +6301,19 @@
       <c r="I6" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="24"/>
+      <c r="J6" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="K6" s="92">
+        <v>100</v>
+      </c>
+      <c r="L6" s="23">
+        <v>49</v>
+      </c>
+      <c r="M6" s="24">
+        <f>ROUND((L6/K6)*100,2)</f>
+        <v>49</v>
+      </c>
       <c r="O6" s="72">
         <v>3</v>
       </c>
@@ -6273,9 +6335,9 @@
       <c r="F7" s="32"/>
       <c r="G7" s="19"/>
       <c r="H7" s="32"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="20"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="13"/>
       <c r="M7" s="14"/>
       <c r="O7" s="73">
@@ -6299,9 +6361,9 @@
       <c r="F8" s="32"/>
       <c r="G8" s="19"/>
       <c r="H8" s="32"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="20"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="13"/>
       <c r="M8" s="14"/>
       <c r="O8" s="72">
@@ -6325,9 +6387,9 @@
       <c r="F9" s="32"/>
       <c r="G9" s="19"/>
       <c r="H9" s="32"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="20"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="12"/>
       <c r="L9" s="13"/>
       <c r="M9" s="14"/>
       <c r="O9" s="51">
@@ -6351,9 +6413,9 @@
       <c r="F10" s="32"/>
       <c r="G10" s="19"/>
       <c r="H10" s="32"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="20"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="13"/>
       <c r="M10" s="14"/>
       <c r="O10" s="51">
@@ -6368,20 +6430,20 @@
       <c r="R10" s="32"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="78">
+      <c r="B11" s="77">
         <v>6</v>
       </c>
-      <c r="C11" s="79"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
       <c r="G11" s="33"/>
-      <c r="H11" s="82"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="81"/>
-      <c r="M11" s="83"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="82"/>
       <c r="O11" s="51">
         <v>8</v>
       </c>
@@ -6394,10 +6456,10 @@
       <c r="R11" s="32"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="157" t="s">
+      <c r="B12" s="149" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="130"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="32" t="s">
         <v>189</v>
       </c>
@@ -6413,13 +6475,21 @@
       <c r="H12" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="I12" s="76" t="s">
+      <c r="I12" s="75" t="s">
         <v>216</v>
       </c>
-      <c r="J12" s="76"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="85"/>
+      <c r="J12" s="75" t="s">
+        <v>225</v>
+      </c>
+      <c r="K12" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="M12" s="84">
+        <v>45318</v>
+      </c>
       <c r="O12" s="51">
         <v>9</v>
       </c>
@@ -6432,7 +6502,7 @@
       <c r="R12" s="32"/>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="84"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="32"/>
       <c r="D13" s="32" t="s">
         <v>190</v>
@@ -6443,9 +6513,13 @@
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
-      <c r="K13" s="84"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75" t="s">
+        <v>226</v>
+      </c>
+      <c r="K13" s="75" t="s">
+        <v>222</v>
+      </c>
       <c r="L13" s="32"/>
       <c r="M13" s="6"/>
       <c r="O13" s="51">
@@ -6460,7 +6534,7 @@
       <c r="R13" s="32"/>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="84"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="32"/>
       <c r="D14" s="32"/>
       <c r="E14" s="32" t="s">
@@ -6469,9 +6543,13 @@
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="84"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75" t="s">
+        <v>228</v>
+      </c>
+      <c r="K14" s="75" t="s">
+        <v>223</v>
+      </c>
       <c r="L14" s="32"/>
       <c r="M14" s="6"/>
       <c r="O14" s="72">
@@ -6486,17 +6564,19 @@
       <c r="R14" s="73"/>
     </row>
     <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="86"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="86"/>
-      <c r="L15" s="87"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87" t="s">
+        <v>227</v>
+      </c>
+      <c r="K15" s="87"/>
+      <c r="L15" s="86"/>
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">

</xml_diff>